<commit_message>
export and import jurisdiction path and group number
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCB49F2-5AF5-A142-A8E8-5EF039400BD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59ED69C-1A0E-CC4F-9B87-B4041F292040}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="223">
   <si>
     <t>First Name</t>
   </si>
@@ -442,9 +442,6 @@
     <t>asgavew</t>
   </si>
   <si>
-    <t>saefase</t>
-  </si>
-  <si>
     <t>asefvae</t>
   </si>
   <si>
@@ -518,6 +515,180 @@
   </si>
   <si>
     <t>sdgafsd</t>
+  </si>
+  <si>
+    <t>Jurisdiction Path</t>
+  </si>
+  <si>
+    <t>Group Number</t>
+  </si>
+  <si>
+    <t>USA, State 2</t>
+  </si>
+  <si>
+    <t>State 1</t>
+  </si>
+  <si>
+    <t>asdfda</t>
+  </si>
+  <si>
+    <t>Lynwood72</t>
+  </si>
+  <si>
+    <t>Ankunding98</t>
+  </si>
+  <si>
+    <t>R968</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Not a state</t>
+  </si>
+  <si>
+    <t>#%#)*$(U@</t>
+  </si>
+  <si>
+    <t>0234990$)(@$!*</t>
+  </si>
+  <si>
+    <t>$@)!(@</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>ZYX</t>
+  </si>
+  <si>
+    <t>asfsdohglkd</t>
+  </si>
+  <si>
+    <t>dfhsgoihalk</t>
+  </si>
+  <si>
+    <t>3%*$R#)(I@SDOh.dsga</t>
+  </si>
+  <si>
+    <t>328u9#)$(U</t>
+  </si>
+  <si>
+    <t>gosdihaflk</t>
+  </si>
+  <si>
+    <t>dsflgh</t>
+  </si>
+  <si>
+    <t>35W*R)#(U#@</t>
+  </si>
+  <si>
+    <t>#($*#</t>
+  </si>
+  <si>
+    <t>#)$(@_1234</t>
+  </si>
+  <si>
+    <t>dghsoiadlkfnve.d</t>
+  </si>
+  <si>
+    <t>asdglkhdngvsro</t>
+  </si>
+  <si>
+    <t>12348oo</t>
+  </si>
+  <si>
+    <t>4325019u</t>
+  </si>
+  <si>
+    <t>21341sdfasbfsd</t>
+  </si>
+  <si>
+    <t>adfsbsdf$#%%$@*</t>
+  </si>
+  <si>
+    <t>01294)($@&amp;)</t>
+  </si>
+  <si>
+    <t>2314r</t>
+  </si>
+  <si>
+    <t>23498</t>
+  </si>
+  <si>
+    <t>#%@#$#(</t>
+  </si>
+  <si>
+    <t>2358)#%</t>
+  </si>
+  <si>
+    <t>234981</t>
+  </si>
+  <si>
+    <t>3253804@$!*@$!(7</t>
+  </si>
+  <si>
+    <t>#958y92oU</t>
+  </si>
+  <si>
+    <t>()(#(%*Y@U(</t>
+  </si>
+  <si>
+    <t>)*#%$(&amp;#*</t>
+  </si>
+  <si>
+    <t>9*SRYH#FNKE</t>
+  </si>
+  <si>
+    <t>(*IOGJDKNLFS</t>
+  </si>
+  <si>
+    <t>08S&amp;DF^(*IYUHJKF&amp;#$#@</t>
+  </si>
+  <si>
+    <t>$%(&amp;*#(*$@P)AFDGS</t>
+  </si>
+  <si>
+    <t>dslfHS#$&amp;@(#YR!</t>
+  </si>
+  <si>
+    <t>(Y*#ORHIFLNWJKSEFH(@#YR)@#*EI</t>
+  </si>
+  <si>
+    <t>!@)#UR$)HTUNP</t>
+  </si>
+  <si>
+    <t>saldanv3wa89rhf23h0@!$(243</t>
+  </si>
+  <si>
+    <t>293840(Ewrf#*</t>
+  </si>
+  <si>
+    <t>(W$*RU)#JFPi</t>
+  </si>
+  <si>
+    <t>)W$*#%R#H)E</t>
+  </si>
+  <si>
+    <t>43238u090DSF#%#</t>
+  </si>
+  <si>
+    <t>#W($&amp;@R</t>
+  </si>
+  <si>
+    <t>01/01/1000</t>
+  </si>
+  <si>
+    <t>05/01/600</t>
+  </si>
+  <si>
+    <t>12/12/1212</t>
+  </si>
+  <si>
+    <t>a39%3</t>
+  </si>
+  <si>
+    <t>USA, State 2, County 1</t>
   </si>
 </sst>
 </file>
@@ -870,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CQ12"/>
+  <dimension ref="A1:CS12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CC1" workbookViewId="0">
-      <selection activeCell="CH2" sqref="CH2"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CF1" workbookViewId="0">
+      <selection activeCell="CQ3" sqref="CQ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -961,21 +1132,23 @@
     <col min="81" max="81" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="82" max="82" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="83" max="83" width="38" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="86" max="86" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="88" max="88" width="14.5" bestFit="1" customWidth="1"/>
     <col min="89" max="89" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="16" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="91" max="91" width="12" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="14.5" bestFit="1" customWidth="1"/>
     <col min="93" max="93" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="94" max="94" width="16" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="12" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="20" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:95" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:97" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1261,8 +1434,14 @@
       <c r="CQ1" t="s">
         <v>122</v>
       </c>
+      <c r="CR1" t="s">
+        <v>165</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>166</v>
+      </c>
     </row>
-    <row r="2" spans="1:95" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:97" x14ac:dyDescent="0.15">
       <c r="E2" t="s">
         <v>125</v>
       </c>
@@ -1354,43 +1533,43 @@
         <v>139</v>
       </c>
       <c r="AV2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AW2" t="s">
         <v>140</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AX2" t="s">
         <v>141</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="AZ2" t="s">
+        <v>185</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>184</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>190</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>189</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BL2" t="s">
         <v>142</v>
       </c>
-      <c r="AZ2" t="s">
-        <v>125</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>125</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>126</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BL2" t="s">
+      <c r="BM2" t="s">
         <v>143</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>144</v>
       </c>
       <c r="BN2" t="s">
         <v>87</v>
@@ -1403,50 +1582,50 @@
         <v>93</v>
       </c>
       <c r="BR2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="BS2" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="BS2" s="1" t="s">
+      <c r="BT2" t="s">
         <v>147</v>
       </c>
-      <c r="BT2" t="s">
+      <c r="BU2" t="s">
         <v>148</v>
       </c>
-      <c r="BU2" t="s">
+      <c r="BV2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BW2" t="s">
         <v>149</v>
       </c>
-      <c r="BV2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BW2" t="s">
+      <c r="BX2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BY2" t="s">
         <v>150</v>
       </c>
-      <c r="BX2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BY2" t="s">
+      <c r="BZ2" t="s">
+        <v>87</v>
+      </c>
+      <c r="CA2" t="s">
         <v>151</v>
       </c>
-      <c r="BZ2" t="s">
-        <v>87</v>
-      </c>
-      <c r="CA2" t="s">
+      <c r="CB2" t="s">
         <v>152</v>
       </c>
-      <c r="CB2" t="s">
+      <c r="CC2" t="s">
+        <v>87</v>
+      </c>
+      <c r="CD2" t="s">
         <v>153</v>
       </c>
-      <c r="CC2" t="s">
-        <v>87</v>
-      </c>
-      <c r="CD2" t="s">
+      <c r="CE2" t="s">
         <v>154</v>
       </c>
-      <c r="CE2" t="s">
+      <c r="CH2" t="s">
         <v>155</v>
       </c>
-      <c r="CH2" t="s">
-        <v>156</v>
-      </c>
       <c r="CJ2" t="s">
         <v>87</v>
       </c>
@@ -1459,8 +1638,14 @@
       <c r="CQ2" t="s">
         <v>87</v>
       </c>
+      <c r="CR2" t="s">
+        <v>168</v>
+      </c>
+      <c r="CS2">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="3" spans="1:95" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:97" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>94</v>
       </c>
@@ -1549,13 +1734,13 @@
         <v>100</v>
       </c>
       <c r="AH3" t="s">
+        <v>156</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ3" t="s">
         <v>157</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>158</v>
       </c>
       <c r="AK3" t="s">
         <v>87</v>
@@ -1636,7 +1821,7 @@
         <v>87</v>
       </c>
       <c r="BO3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="BP3" t="s">
         <v>87</v>
@@ -1690,25 +1875,25 @@
         <v>123</v>
       </c>
       <c r="CI3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="CJ3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="CK3" t="s">
+        <v>158</v>
+      </c>
+      <c r="CL3" t="s">
         <v>159</v>
       </c>
-      <c r="CL3" t="s">
+      <c r="CM3" t="s">
+        <v>162</v>
+      </c>
+      <c r="CN3" t="s">
+        <v>161</v>
+      </c>
+      <c r="CO3" t="s">
         <v>160</v>
-      </c>
-      <c r="CM3" t="s">
-        <v>163</v>
-      </c>
-      <c r="CN3" t="s">
-        <v>162</v>
-      </c>
-      <c r="CO3" t="s">
-        <v>161</v>
       </c>
       <c r="CP3" t="s">
         <v>125</v>
@@ -1716,24 +1901,253 @@
       <c r="CQ3" t="s">
         <v>126</v>
       </c>
+      <c r="CR3" t="s">
+        <v>167</v>
+      </c>
+      <c r="CS3" t="s">
+        <v>169</v>
+      </c>
     </row>
-    <row r="4" spans="1:95" x14ac:dyDescent="0.15">
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="BT4" s="1"/>
-      <c r="BU4" s="1"/>
-      <c r="BW4" s="1"/>
-      <c r="BX4" s="1"/>
-      <c r="BY4" s="1"/>
-      <c r="CA4" s="1"/>
-      <c r="CB4" s="1"/>
-      <c r="CD4" s="1"/>
+    <row r="4" spans="1:97" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E4" t="s">
+        <v>173</v>
+      </c>
+      <c r="R4" t="s">
+        <v>87</v>
+      </c>
+      <c r="S4">
+        <v>887</v>
+      </c>
+      <c r="T4">
+        <v>1234</v>
+      </c>
+      <c r="U4" t="s">
+        <v>174</v>
+      </c>
+      <c r="V4" t="s">
+        <v>87</v>
+      </c>
+      <c r="W4">
+        <v>381942349</v>
+      </c>
+      <c r="X4">
+        <v>123</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF4">
+        <v>94219</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>175</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>176</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>177</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR4">
+        <v>2130</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>178</v>
+      </c>
+      <c r="AT4">
+        <v>324899</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>179</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AW4">
+        <v>12451324</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>182</v>
+      </c>
+      <c r="AY4">
+        <v>124394</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>186</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>183</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BG4" t="s">
+        <v>187</v>
+      </c>
+      <c r="BH4" t="s">
+        <v>188</v>
+      </c>
+      <c r="BI4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BJ4" t="s">
+        <v>191</v>
+      </c>
+      <c r="BK4" t="s">
+        <v>192</v>
+      </c>
+      <c r="BL4" t="s">
+        <v>193</v>
+      </c>
+      <c r="BM4" t="s">
+        <v>194</v>
+      </c>
+      <c r="BN4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BO4" t="s">
+        <v>195</v>
+      </c>
+      <c r="BP4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BQ4" t="s">
+        <v>196</v>
+      </c>
+      <c r="BR4" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="BS4" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="BT4" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="BU4" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="BV4" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="BW4" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="BX4" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="BY4" t="s">
+        <v>204</v>
+      </c>
+      <c r="BZ4" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="CA4" t="s">
+        <v>206</v>
+      </c>
+      <c r="CB4" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="CC4" t="s">
+        <v>208</v>
+      </c>
+      <c r="CD4" t="s">
+        <v>209</v>
+      </c>
+      <c r="CE4" t="s">
+        <v>210</v>
+      </c>
+      <c r="CF4" t="s">
+        <v>211</v>
+      </c>
+      <c r="CG4" t="s">
+        <v>212</v>
+      </c>
+      <c r="CH4" t="s">
+        <v>213</v>
+      </c>
+      <c r="CI4" t="s">
+        <v>214</v>
+      </c>
+      <c r="CJ4" s="3">
+        <v>44124</v>
+      </c>
+      <c r="CK4" t="s">
+        <v>215</v>
+      </c>
+      <c r="CL4" t="s">
+        <v>216</v>
+      </c>
+      <c r="CM4" t="s">
+        <v>217</v>
+      </c>
+      <c r="CN4" t="s">
+        <v>218</v>
+      </c>
+      <c r="CO4" t="s">
+        <v>219</v>
+      </c>
+      <c r="CP4" t="s">
+        <v>220</v>
+      </c>
+      <c r="CQ4" t="s">
+        <v>221</v>
+      </c>
+      <c r="CR4" t="s">
+        <v>222</v>
+      </c>
+      <c r="CS4">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="5" spans="1:95" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:97" x14ac:dyDescent="0.15">
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1746,11 +2160,11 @@
       <c r="CD5" s="1"/>
       <c r="CH5" s="2"/>
     </row>
-    <row r="6" spans="1:95" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:97" x14ac:dyDescent="0.15">
       <c r="CK6" s="2"/>
       <c r="CL6" s="3"/>
     </row>
-    <row r="7" spans="1:95" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:97" x14ac:dyDescent="0.15">
       <c r="D7" s="2"/>
       <c r="BL7" s="2"/>
       <c r="BM7" s="2"/>
@@ -1763,7 +2177,7 @@
       <c r="CO7" s="2"/>
       <c r="CP7" s="3"/>
     </row>
-    <row r="8" spans="1:95" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:97" x14ac:dyDescent="0.15">
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1780,7 +2194,7 @@
       <c r="CB8" s="1"/>
       <c r="CD8" s="1"/>
     </row>
-    <row r="9" spans="1:95" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:97" x14ac:dyDescent="0.15">
       <c r="D9" s="3"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1797,7 +2211,7 @@
       <c r="CC9" s="1"/>
       <c r="CD9" s="1"/>
     </row>
-    <row r="10" spans="1:95" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:97" x14ac:dyDescent="0.15">
       <c r="AZ10" s="2"/>
       <c r="BE10" s="2"/>
       <c r="BO10" s="3"/>
@@ -1806,7 +2220,7 @@
       <c r="CO10" s="3"/>
       <c r="CP10" s="2"/>
     </row>
-    <row r="12" spans="1:95" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:97" x14ac:dyDescent="0.15">
       <c r="D12" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change field name to assigned user
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59ED69C-1A0E-CC4F-9B87-B4041F292040}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE38393-FA1A-B04D-BEC3-85C27B78A9E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -520,9 +520,6 @@
     <t>Jurisdiction Path</t>
   </si>
   <si>
-    <t>Group Number</t>
-  </si>
-  <si>
     <t>USA, State 2</t>
   </si>
   <si>
@@ -689,6 +686,9 @@
   </si>
   <si>
     <t>USA, State 2, County 1</t>
+  </si>
+  <si>
+    <t>Assigned User</t>
   </si>
 </sst>
 </file>
@@ -1043,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CS12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CF1" workbookViewId="0">
-      <selection activeCell="CQ3" sqref="CQ3"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CG1" workbookViewId="0">
+      <selection activeCell="CS4" sqref="CS4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1438,7 +1438,7 @@
         <v>165</v>
       </c>
       <c r="CS1" t="s">
-        <v>166</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.15">
@@ -1533,7 +1533,7 @@
         <v>139</v>
       </c>
       <c r="AV2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AW2" t="s">
         <v>140</v>
@@ -1542,22 +1542,22 @@
         <v>141</v>
       </c>
       <c r="AZ2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="BE2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="BF2" t="s">
         <v>87</v>
       </c>
       <c r="BG2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="BH2" t="s">
         <v>87</v>
       </c>
       <c r="BI2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BJ2" t="s">
         <v>87</v>
@@ -1639,7 +1639,7 @@
         <v>87</v>
       </c>
       <c r="CR2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="CS2">
         <v>-1</v>
@@ -1902,24 +1902,24 @@
         <v>126</v>
       </c>
       <c r="CR3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="CS3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:97" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C4" t="s">
         <v>170</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>171</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>172</v>
-      </c>
-      <c r="E4" t="s">
-        <v>173</v>
       </c>
       <c r="R4" t="s">
         <v>87</v>
@@ -1931,7 +1931,7 @@
         <v>1234</v>
       </c>
       <c r="U4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="V4" t="s">
         <v>87</v>
@@ -1964,16 +1964,16 @@
         <v>94219</v>
       </c>
       <c r="AG4" t="s">
+        <v>174</v>
+      </c>
+      <c r="AH4" t="s">
         <v>175</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ4" t="s">
         <v>176</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>177</v>
       </c>
       <c r="AK4" t="s">
         <v>87</v>
@@ -2000,148 +2000,148 @@
         <v>2130</v>
       </c>
       <c r="AS4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AT4">
         <v>324899</v>
       </c>
       <c r="AU4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AV4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AW4">
         <v>12451324</v>
       </c>
       <c r="AX4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AY4">
         <v>124394</v>
       </c>
       <c r="AZ4" t="s">
+        <v>185</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>182</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BG4" t="s">
         <v>186</v>
       </c>
-      <c r="BE4" t="s">
-        <v>183</v>
-      </c>
-      <c r="BF4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BG4" t="s">
+      <c r="BH4" t="s">
         <v>187</v>
       </c>
-      <c r="BH4" t="s">
-        <v>188</v>
-      </c>
       <c r="BI4" t="s">
         <v>87</v>
       </c>
       <c r="BJ4" t="s">
+        <v>190</v>
+      </c>
+      <c r="BK4" t="s">
         <v>191</v>
       </c>
-      <c r="BK4" t="s">
+      <c r="BL4" t="s">
         <v>192</v>
       </c>
-      <c r="BL4" t="s">
+      <c r="BM4" t="s">
         <v>193</v>
       </c>
-      <c r="BM4" t="s">
+      <c r="BN4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BO4" t="s">
         <v>194</v>
       </c>
-      <c r="BN4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BO4" t="s">
+      <c r="BP4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BQ4" t="s">
         <v>195</v>
       </c>
-      <c r="BP4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BQ4" t="s">
+      <c r="BR4" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="BR4" s="1" t="s">
+      <c r="BS4" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="BS4" s="1" t="s">
+      <c r="BT4" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="BT4" s="1" t="s">
+      <c r="BU4" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="BU4" s="1" t="s">
+      <c r="BV4" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="BV4" s="1" t="s">
+      <c r="BW4" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="BW4" s="1" t="s">
+      <c r="BX4" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="BX4" s="1" t="s">
+      <c r="BY4" t="s">
         <v>203</v>
       </c>
-      <c r="BY4" t="s">
+      <c r="BZ4" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="BZ4" s="1" t="s">
+      <c r="CA4" t="s">
         <v>205</v>
       </c>
-      <c r="CA4" t="s">
+      <c r="CB4" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="CB4" s="1" t="s">
+      <c r="CC4" t="s">
         <v>207</v>
       </c>
-      <c r="CC4" t="s">
+      <c r="CD4" t="s">
         <v>208</v>
       </c>
-      <c r="CD4" t="s">
+      <c r="CE4" t="s">
         <v>209</v>
       </c>
-      <c r="CE4" t="s">
+      <c r="CF4" t="s">
         <v>210</v>
       </c>
-      <c r="CF4" t="s">
+      <c r="CG4" t="s">
         <v>211</v>
       </c>
-      <c r="CG4" t="s">
+      <c r="CH4" t="s">
         <v>212</v>
       </c>
-      <c r="CH4" t="s">
+      <c r="CI4" t="s">
         <v>213</v>
-      </c>
-      <c r="CI4" t="s">
-        <v>214</v>
       </c>
       <c r="CJ4" s="3">
         <v>44124</v>
       </c>
       <c r="CK4" t="s">
+        <v>214</v>
+      </c>
+      <c r="CL4" t="s">
         <v>215</v>
       </c>
-      <c r="CL4" t="s">
+      <c r="CM4" t="s">
         <v>216</v>
       </c>
-      <c r="CM4" t="s">
+      <c r="CN4" t="s">
         <v>217</v>
       </c>
-      <c r="CN4" t="s">
+      <c r="CO4" t="s">
         <v>218</v>
       </c>
-      <c r="CO4" t="s">
+      <c r="CP4" t="s">
         <v>219</v>
       </c>
-      <c r="CP4" t="s">
+      <c r="CQ4" t="s">
         <v>220</v>
       </c>
-      <c r="CQ4" t="s">
+      <c r="CR4" t="s">
         <v>221</v>
-      </c>
-      <c r="CR4" t="s">
-        <v>222</v>
       </c>
       <c r="CS4">
         <v>5.5</v>

</xml_diff>

<commit_message>
update import tests to include jurisdiction path and assigned user
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE38393-FA1A-B04D-BEC3-85C27B78A9E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7380A14C-8562-804E-A053-78BF28C9A949}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitorees" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="224">
   <si>
     <t>First Name</t>
   </si>
@@ -689,6 +689,9 @@
   </si>
   <si>
     <t>Assigned User</t>
+  </si>
+  <si>
+    <t>ahewfsvjdnzk</t>
   </si>
 </sst>
 </file>
@@ -1043,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CS12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CG1" workbookViewId="0">
-      <selection activeCell="CS4" sqref="CS4"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1052,7 +1055,7 @@
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
@@ -1646,267 +1649,10 @@
       </c>
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G3" t="s">
-        <v>85</v>
-      </c>
-      <c r="H3" t="s">
-        <v>85</v>
-      </c>
-      <c r="I3" t="s">
-        <v>86</v>
-      </c>
-      <c r="J3" t="s">
-        <v>85</v>
-      </c>
-      <c r="K3" t="s">
-        <v>98</v>
-      </c>
-      <c r="M3" t="s">
-        <v>87</v>
-      </c>
-      <c r="N3" t="s">
-        <v>85</v>
-      </c>
-      <c r="O3" t="s">
-        <v>87</v>
-      </c>
-      <c r="R3" t="s">
-        <v>87</v>
-      </c>
-      <c r="S3" t="s">
-        <v>99</v>
-      </c>
-      <c r="T3" t="s">
-        <v>100</v>
-      </c>
-      <c r="U3" t="s">
-        <v>125</v>
-      </c>
-      <c r="V3" t="s">
-        <v>87</v>
-      </c>
-      <c r="W3" t="s">
-        <v>101</v>
-      </c>
-      <c r="X3" t="s">
-        <v>128</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>99</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>100</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>156</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>157</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>129</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>88</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>88</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>127</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE3" t="s">
-        <v>91</v>
-      </c>
-      <c r="BF3" t="s">
-        <v>87</v>
-      </c>
-      <c r="BG3" t="s">
-        <v>104</v>
-      </c>
-      <c r="BH3" t="s">
-        <v>105</v>
-      </c>
-      <c r="BI3" t="s">
-        <v>87</v>
-      </c>
-      <c r="BJ3" t="s">
-        <v>106</v>
-      </c>
-      <c r="BK3" t="s">
-        <v>107</v>
-      </c>
-      <c r="BL3" t="s">
-        <v>108</v>
-      </c>
-      <c r="BM3" t="s">
-        <v>109</v>
-      </c>
-      <c r="BN3" t="s">
-        <v>87</v>
-      </c>
-      <c r="BO3" t="s">
-        <v>144</v>
-      </c>
-      <c r="BP3" t="s">
-        <v>87</v>
-      </c>
-      <c r="BQ3" t="s">
-        <v>110</v>
-      </c>
-      <c r="BR3" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="BS3" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="BT3" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="BU3" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="BV3" t="s">
-        <v>87</v>
-      </c>
-      <c r="BW3" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="BX3" t="s">
-        <v>87</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>85</v>
-      </c>
-      <c r="BZ3" t="s">
-        <v>87</v>
-      </c>
-      <c r="CA3" t="s">
-        <v>85</v>
-      </c>
-      <c r="CB3" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="CC3" t="s">
-        <v>87</v>
-      </c>
-      <c r="CD3" t="s">
-        <v>111</v>
-      </c>
-      <c r="CE3" t="s">
-        <v>112</v>
-      </c>
-      <c r="CH3" t="s">
-        <v>123</v>
-      </c>
-      <c r="CI3" t="s">
-        <v>164</v>
-      </c>
-      <c r="CJ3" t="s">
-        <v>163</v>
-      </c>
-      <c r="CK3" t="s">
-        <v>158</v>
-      </c>
-      <c r="CL3" t="s">
-        <v>159</v>
-      </c>
-      <c r="CM3" t="s">
-        <v>162</v>
-      </c>
-      <c r="CN3" t="s">
-        <v>161</v>
-      </c>
-      <c r="CO3" t="s">
-        <v>160</v>
-      </c>
-      <c r="CP3" t="s">
-        <v>125</v>
-      </c>
-      <c r="CQ3" t="s">
-        <v>126</v>
-      </c>
-      <c r="CR3" t="s">
-        <v>166</v>
-      </c>
-      <c r="CS3" t="s">
-        <v>168</v>
-      </c>
+      <c r="BT3" s="1"/>
+      <c r="BU3" s="1"/>
+      <c r="BW3" s="1"/>
+      <c r="CB3" s="1"/>
     </row>
     <row r="4" spans="1:97" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
@@ -2148,21 +1894,273 @@
       </c>
     </row>
     <row r="5" spans="1:97" x14ac:dyDescent="0.15">
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="BY5" s="1"/>
-      <c r="CA5" s="1"/>
-      <c r="CD5" s="1"/>
-      <c r="CH5" s="2"/>
+      <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" t="s">
+        <v>223</v>
+      </c>
+      <c r="E5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" t="s">
+        <v>85</v>
+      </c>
+      <c r="K5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M5" t="s">
+        <v>87</v>
+      </c>
+      <c r="N5" t="s">
+        <v>85</v>
+      </c>
+      <c r="O5" t="s">
+        <v>87</v>
+      </c>
+      <c r="R5" t="s">
+        <v>87</v>
+      </c>
+      <c r="S5" t="s">
+        <v>99</v>
+      </c>
+      <c r="T5" t="s">
+        <v>100</v>
+      </c>
+      <c r="U5" t="s">
+        <v>125</v>
+      </c>
+      <c r="V5" t="s">
+        <v>87</v>
+      </c>
+      <c r="W5" t="s">
+        <v>101</v>
+      </c>
+      <c r="X5" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>99</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>156</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>157</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>129</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>89</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>127</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>102</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>103</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE5" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>87</v>
+      </c>
+      <c r="BG5" t="s">
+        <v>104</v>
+      </c>
+      <c r="BH5" t="s">
+        <v>105</v>
+      </c>
+      <c r="BI5" t="s">
+        <v>87</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>106</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>107</v>
+      </c>
+      <c r="BL5" t="s">
+        <v>108</v>
+      </c>
+      <c r="BM5" t="s">
+        <v>109</v>
+      </c>
+      <c r="BN5" t="s">
+        <v>87</v>
+      </c>
+      <c r="BO5" t="s">
+        <v>144</v>
+      </c>
+      <c r="BP5" t="s">
+        <v>87</v>
+      </c>
+      <c r="BQ5" t="s">
+        <v>110</v>
+      </c>
+      <c r="BR5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BS5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BT5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="BU5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="BV5" t="s">
+        <v>87</v>
+      </c>
+      <c r="BW5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="BX5" t="s">
+        <v>87</v>
+      </c>
+      <c r="BY5" t="s">
+        <v>85</v>
+      </c>
+      <c r="BZ5" t="s">
+        <v>87</v>
+      </c>
+      <c r="CA5" t="s">
+        <v>85</v>
+      </c>
+      <c r="CB5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="CC5" t="s">
+        <v>87</v>
+      </c>
+      <c r="CD5" t="s">
+        <v>111</v>
+      </c>
+      <c r="CE5" t="s">
+        <v>112</v>
+      </c>
+      <c r="CH5" t="s">
+        <v>123</v>
+      </c>
+      <c r="CI5" t="s">
+        <v>164</v>
+      </c>
+      <c r="CJ5" t="s">
+        <v>163</v>
+      </c>
+      <c r="CK5" t="s">
+        <v>158</v>
+      </c>
+      <c r="CL5" t="s">
+        <v>159</v>
+      </c>
+      <c r="CM5" t="s">
+        <v>162</v>
+      </c>
+      <c r="CN5" t="s">
+        <v>161</v>
+      </c>
+      <c r="CO5" t="s">
+        <v>160</v>
+      </c>
+      <c r="CP5" t="s">
+        <v>125</v>
+      </c>
+      <c r="CQ5" t="s">
+        <v>126</v>
+      </c>
+      <c r="CR5" t="s">
+        <v>166</v>
+      </c>
+      <c r="CS5" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="6" spans="1:97" x14ac:dyDescent="0.15">
-      <c r="CK6" s="2"/>
-      <c r="CL6" s="3"/>
+      <c r="BT6" s="1"/>
+      <c r="BU6" s="1"/>
+      <c r="BW6" s="1"/>
+      <c r="CB6" s="1"/>
     </row>
     <row r="7" spans="1:97" x14ac:dyDescent="0.15">
       <c r="D7" s="2"/>

</xml_diff>

<commit_message>
update sara alert format and data table filter and column labels, bugfixes, improved import validation messages, improved monitoring actions ui
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7380A14C-8562-804E-A053-78BF28C9A949}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC55BF7-17DA-004C-BDAF-D4A89007973A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="222">
   <si>
     <t>First Name</t>
   </si>
@@ -517,15 +517,6 @@
     <t>sdgafsd</t>
   </si>
   <si>
-    <t>Jurisdiction Path</t>
-  </si>
-  <si>
-    <t>USA, State 2</t>
-  </si>
-  <si>
-    <t>State 1</t>
-  </si>
-  <si>
     <t>asdfda</t>
   </si>
   <si>
@@ -685,13 +676,16 @@
     <t>a39%3</t>
   </si>
   <si>
-    <t>USA, State 2, County 1</t>
-  </si>
-  <si>
     <t>Assigned User</t>
   </si>
   <si>
     <t>ahewfsvjdnzk</t>
+  </si>
+  <si>
+    <t>Full Assigned Jurisdiction Path</t>
+  </si>
+  <si>
+    <t>(*#RY$HNlsDFk</t>
   </si>
 </sst>
 </file>
@@ -1046,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CS12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CI1" workbookViewId="0">
+      <selection activeCell="CR5" sqref="CR5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1147,7 +1141,7 @@
     <col min="93" max="93" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="94" max="94" width="16" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="12" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="20" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="97" max="97" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1438,10 +1432,10 @@
         <v>122</v>
       </c>
       <c r="CR1" t="s">
-        <v>165</v>
+        <v>220</v>
       </c>
       <c r="CS1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.15">
@@ -1536,7 +1530,7 @@
         <v>139</v>
       </c>
       <c r="AV2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="AW2" t="s">
         <v>140</v>
@@ -1545,22 +1539,22 @@
         <v>141</v>
       </c>
       <c r="AZ2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="BE2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="BF2" t="s">
         <v>87</v>
       </c>
       <c r="BG2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="BH2" t="s">
         <v>87</v>
       </c>
       <c r="BI2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="BJ2" t="s">
         <v>87</v>
@@ -1642,7 +1636,7 @@
         <v>87</v>
       </c>
       <c r="CR2" t="s">
-        <v>167</v>
+        <v>125</v>
       </c>
       <c r="CS2">
         <v>-1</v>
@@ -1653,19 +1647,22 @@
       <c r="BU3" s="1"/>
       <c r="BW3" s="1"/>
       <c r="CB3" s="1"/>
+      <c r="CR3" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="4" spans="1:97" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E4" t="s">
         <v>169</v>
-      </c>
-      <c r="C4" t="s">
-        <v>170</v>
-      </c>
-      <c r="D4" t="s">
-        <v>171</v>
-      </c>
-      <c r="E4" t="s">
-        <v>172</v>
       </c>
       <c r="R4" t="s">
         <v>87</v>
@@ -1677,7 +1674,7 @@
         <v>1234</v>
       </c>
       <c r="U4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="V4" t="s">
         <v>87</v>
@@ -1710,16 +1707,16 @@
         <v>94219</v>
       </c>
       <c r="AG4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AH4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AI4" t="s">
         <v>87</v>
       </c>
       <c r="AJ4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AK4" t="s">
         <v>87</v>
@@ -1746,145 +1743,145 @@
         <v>2130</v>
       </c>
       <c r="AS4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AT4">
         <v>324899</v>
       </c>
       <c r="AU4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="AV4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AW4">
         <v>12451324</v>
       </c>
       <c r="AX4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="AY4">
         <v>124394</v>
       </c>
       <c r="AZ4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="BE4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="BF4" t="s">
         <v>87</v>
       </c>
       <c r="BG4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="BH4" t="s">
+        <v>184</v>
+      </c>
+      <c r="BI4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BJ4" t="s">
         <v>187</v>
       </c>
-      <c r="BI4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BJ4" t="s">
+      <c r="BK4" t="s">
+        <v>188</v>
+      </c>
+      <c r="BL4" t="s">
+        <v>189</v>
+      </c>
+      <c r="BM4" t="s">
         <v>190</v>
       </c>
-      <c r="BK4" t="s">
+      <c r="BN4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BO4" t="s">
         <v>191</v>
       </c>
-      <c r="BL4" t="s">
+      <c r="BP4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BQ4" t="s">
         <v>192</v>
       </c>
-      <c r="BM4" t="s">
+      <c r="BR4" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BN4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BO4" t="s">
+      <c r="BS4" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BP4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BQ4" t="s">
+      <c r="BT4" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="BR4" s="1" t="s">
+      <c r="BU4" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="BS4" s="1" t="s">
+      <c r="BV4" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="BT4" s="1" t="s">
+      <c r="BW4" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="BU4" s="1" t="s">
+      <c r="BX4" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="BV4" s="1" t="s">
+      <c r="BY4" t="s">
         <v>200</v>
       </c>
-      <c r="BW4" s="1" t="s">
+      <c r="BZ4" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="BX4" s="1" t="s">
+      <c r="CA4" t="s">
         <v>202</v>
       </c>
-      <c r="BY4" t="s">
+      <c r="CB4" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="BZ4" s="1" t="s">
+      <c r="CC4" t="s">
         <v>204</v>
       </c>
-      <c r="CA4" t="s">
+      <c r="CD4" t="s">
         <v>205</v>
       </c>
-      <c r="CB4" s="1" t="s">
+      <c r="CE4" t="s">
         <v>206</v>
       </c>
-      <c r="CC4" t="s">
+      <c r="CF4" t="s">
         <v>207</v>
       </c>
-      <c r="CD4" t="s">
+      <c r="CG4" t="s">
         <v>208</v>
       </c>
-      <c r="CE4" t="s">
+      <c r="CH4" t="s">
         <v>209</v>
       </c>
-      <c r="CF4" t="s">
+      <c r="CI4" t="s">
         <v>210</v>
-      </c>
-      <c r="CG4" t="s">
-        <v>211</v>
-      </c>
-      <c r="CH4" t="s">
-        <v>212</v>
-      </c>
-      <c r="CI4" t="s">
-        <v>213</v>
       </c>
       <c r="CJ4" s="3">
         <v>44124</v>
       </c>
       <c r="CK4" t="s">
+        <v>211</v>
+      </c>
+      <c r="CL4" t="s">
+        <v>212</v>
+      </c>
+      <c r="CM4" t="s">
+        <v>213</v>
+      </c>
+      <c r="CN4" t="s">
         <v>214</v>
       </c>
-      <c r="CL4" t="s">
+      <c r="CO4" t="s">
         <v>215</v>
       </c>
-      <c r="CM4" t="s">
+      <c r="CP4" t="s">
         <v>216</v>
       </c>
-      <c r="CN4" t="s">
+      <c r="CQ4" t="s">
         <v>217</v>
-      </c>
-      <c r="CO4" t="s">
-        <v>218</v>
-      </c>
-      <c r="CP4" t="s">
-        <v>219</v>
-      </c>
-      <c r="CQ4" t="s">
-        <v>220</v>
       </c>
       <c r="CR4" t="s">
         <v>221</v>
@@ -1904,7 +1901,7 @@
         <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E5" t="s">
         <v>97</v>
@@ -2149,11 +2146,11 @@
       <c r="CQ5" t="s">
         <v>126</v>
       </c>
-      <c r="CR5" t="s">
-        <v>166</v>
+      <c r="CR5">
+        <v>123</v>
       </c>
       <c r="CS5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:97" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
fix import date format
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC55BF7-17DA-004C-BDAF-D4A89007973A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6F9457-4E41-8841-9044-F6B58A241698}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="224">
   <si>
     <t>First Name</t>
   </si>
@@ -526,9 +526,6 @@
     <t>Ankunding98</t>
   </si>
   <si>
-    <t>R968</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -686,6 +683,15 @@
   </si>
   <si>
     <t>(*#RY$HNlsDFk</t>
+  </si>
+  <si>
+    <t>06/05/2005</t>
+  </si>
+  <si>
+    <t>10/05/05</t>
+  </si>
+  <si>
+    <t>2005-05-42</t>
   </si>
 </sst>
 </file>
@@ -1040,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CS12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CI1" workbookViewId="0">
-      <selection activeCell="CR5" sqref="CR5"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1432,13 +1438,16 @@
         <v>122</v>
       </c>
       <c r="CR1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="CS1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.15">
+      <c r="D2" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="E2" t="s">
         <v>125</v>
       </c>
@@ -1530,7 +1539,7 @@
         <v>139</v>
       </c>
       <c r="AV2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AW2" t="s">
         <v>140</v>
@@ -1539,22 +1548,22 @@
         <v>141</v>
       </c>
       <c r="AZ2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BE2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="BF2" t="s">
         <v>87</v>
       </c>
       <c r="BG2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="BH2" t="s">
         <v>87</v>
       </c>
       <c r="BI2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="BJ2" t="s">
         <v>87</v>
@@ -1643,6 +1652,9 @@
       </c>
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.15">
+      <c r="D3" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="BT3" s="1"/>
       <c r="BU3" s="1"/>
       <c r="BW3" s="1"/>
@@ -1659,10 +1671,10 @@
         <v>167</v>
       </c>
       <c r="D4" t="s">
+        <v>223</v>
+      </c>
+      <c r="E4" t="s">
         <v>168</v>
-      </c>
-      <c r="E4" t="s">
-        <v>169</v>
       </c>
       <c r="R4" t="s">
         <v>87</v>
@@ -1674,7 +1686,7 @@
         <v>1234</v>
       </c>
       <c r="U4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="V4" t="s">
         <v>87</v>
@@ -1707,16 +1719,16 @@
         <v>94219</v>
       </c>
       <c r="AG4" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH4" t="s">
         <v>171</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ4" t="s">
         <v>172</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>173</v>
       </c>
       <c r="AK4" t="s">
         <v>87</v>
@@ -1743,148 +1755,148 @@
         <v>2130</v>
       </c>
       <c r="AS4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AT4">
         <v>324899</v>
       </c>
       <c r="AU4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AV4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AW4">
         <v>12451324</v>
       </c>
       <c r="AX4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AY4">
         <v>124394</v>
       </c>
       <c r="AZ4" t="s">
+        <v>181</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>178</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BG4" t="s">
         <v>182</v>
       </c>
-      <c r="BE4" t="s">
-        <v>179</v>
-      </c>
-      <c r="BF4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BG4" t="s">
+      <c r="BH4" t="s">
         <v>183</v>
       </c>
-      <c r="BH4" t="s">
-        <v>184</v>
-      </c>
       <c r="BI4" t="s">
         <v>87</v>
       </c>
       <c r="BJ4" t="s">
+        <v>186</v>
+      </c>
+      <c r="BK4" t="s">
         <v>187</v>
       </c>
-      <c r="BK4" t="s">
+      <c r="BL4" t="s">
         <v>188</v>
       </c>
-      <c r="BL4" t="s">
+      <c r="BM4" t="s">
         <v>189</v>
       </c>
-      <c r="BM4" t="s">
+      <c r="BN4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BO4" t="s">
         <v>190</v>
       </c>
-      <c r="BN4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BO4" t="s">
+      <c r="BP4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BQ4" t="s">
         <v>191</v>
       </c>
-      <c r="BP4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BQ4" t="s">
+      <c r="BR4" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="BR4" s="1" t="s">
+      <c r="BS4" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BS4" s="1" t="s">
+      <c r="BT4" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BT4" s="1" t="s">
+      <c r="BU4" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="BU4" s="1" t="s">
+      <c r="BV4" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="BV4" s="1" t="s">
+      <c r="BW4" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="BW4" s="1" t="s">
+      <c r="BX4" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="BX4" s="1" t="s">
+      <c r="BY4" t="s">
         <v>199</v>
       </c>
-      <c r="BY4" t="s">
+      <c r="BZ4" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="BZ4" s="1" t="s">
+      <c r="CA4" t="s">
         <v>201</v>
       </c>
-      <c r="CA4" t="s">
+      <c r="CB4" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="CB4" s="1" t="s">
+      <c r="CC4" t="s">
         <v>203</v>
       </c>
-      <c r="CC4" t="s">
+      <c r="CD4" t="s">
         <v>204</v>
       </c>
-      <c r="CD4" t="s">
+      <c r="CE4" t="s">
         <v>205</v>
       </c>
-      <c r="CE4" t="s">
+      <c r="CF4" t="s">
         <v>206</v>
       </c>
-      <c r="CF4" t="s">
+      <c r="CG4" t="s">
         <v>207</v>
       </c>
-      <c r="CG4" t="s">
+      <c r="CH4" t="s">
         <v>208</v>
       </c>
-      <c r="CH4" t="s">
+      <c r="CI4" t="s">
         <v>209</v>
-      </c>
-      <c r="CI4" t="s">
-        <v>210</v>
       </c>
       <c r="CJ4" s="3">
         <v>44124</v>
       </c>
       <c r="CK4" t="s">
+        <v>210</v>
+      </c>
+      <c r="CL4" t="s">
         <v>211</v>
       </c>
-      <c r="CL4" t="s">
+      <c r="CM4" t="s">
         <v>212</v>
       </c>
-      <c r="CM4" t="s">
+      <c r="CN4" t="s">
         <v>213</v>
       </c>
-      <c r="CN4" t="s">
+      <c r="CO4" t="s">
         <v>214</v>
       </c>
-      <c r="CO4" t="s">
+      <c r="CP4" t="s">
         <v>215</v>
       </c>
-      <c r="CP4" t="s">
+      <c r="CQ4" t="s">
         <v>216</v>
       </c>
-      <c r="CQ4" t="s">
-        <v>217</v>
-      </c>
       <c r="CR4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="CS4">
         <v>5.5</v>
@@ -1901,7 +1913,7 @@
         <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E5" t="s">
         <v>97</v>
@@ -2221,5 +2233,8 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
+  <ignoredErrors>
+    <ignoredError sqref="D3" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
improve importer to remove whitespace and caps sensitivity
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA/SaraAlert/test/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA-ALERT/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6F9457-4E41-8841-9044-F6B58A241698}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7260ABE2-BDE7-DF47-BF66-000BB3370EDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="223">
   <si>
     <t>First Name</t>
   </si>
@@ -407,9 +407,6 @@
   </si>
   <si>
     <t>County 1</t>
-  </si>
-  <si>
-    <t>SMS Texted Weblink</t>
   </si>
   <si>
     <t>wefsas</t>
@@ -1046,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CS12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="AM1" workbookViewId="0">
+      <selection activeCell="AR6" sqref="AR6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1438,15 +1435,15 @@
         <v>122</v>
       </c>
       <c r="CR1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="CS1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.15">
       <c r="D2" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E2" t="s">
         <v>125</v>
@@ -1455,127 +1452,127 @@
         <v>126</v>
       </c>
       <c r="G2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" t="s">
         <v>130</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J2" t="s">
         <v>131</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" t="s">
         <v>134</v>
       </c>
-      <c r="J2" t="s">
-        <v>132</v>
-      </c>
-      <c r="K2" t="s">
-        <v>133</v>
-      </c>
-      <c r="M2" t="s">
-        <v>87</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
+        <v>87</v>
+      </c>
+      <c r="R2" t="s">
+        <v>87</v>
+      </c>
+      <c r="X2" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR2" t="s">
         <v>135</v>
       </c>
-      <c r="O2" t="s">
-        <v>87</v>
-      </c>
-      <c r="R2" t="s">
-        <v>87</v>
-      </c>
-      <c r="X2" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>136</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
         <v>137</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AU2" t="s">
         <v>138</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AV2" t="s">
+        <v>174</v>
+      </c>
+      <c r="AW2" t="s">
         <v>139</v>
       </c>
-      <c r="AV2" t="s">
-        <v>175</v>
-      </c>
-      <c r="AW2" t="s">
+      <c r="AX2" t="s">
         <v>140</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="AZ2" t="s">
+        <v>179</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>178</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>184</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>183</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BL2" t="s">
         <v>141</v>
       </c>
-      <c r="AZ2" t="s">
-        <v>180</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>179</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>185</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>184</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BL2" t="s">
+      <c r="BM2" t="s">
         <v>142</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>143</v>
       </c>
       <c r="BN2" t="s">
         <v>87</v>
@@ -1588,49 +1585,49 @@
         <v>93</v>
       </c>
       <c r="BR2" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="BS2" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="BS2" s="1" t="s">
+      <c r="BT2" t="s">
         <v>146</v>
       </c>
-      <c r="BT2" t="s">
+      <c r="BU2" t="s">
         <v>147</v>
       </c>
-      <c r="BU2" t="s">
+      <c r="BV2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BW2" t="s">
         <v>148</v>
       </c>
-      <c r="BV2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BW2" t="s">
+      <c r="BX2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BY2" t="s">
         <v>149</v>
       </c>
-      <c r="BX2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BY2" t="s">
+      <c r="BZ2" t="s">
+        <v>87</v>
+      </c>
+      <c r="CA2" t="s">
         <v>150</v>
       </c>
-      <c r="BZ2" t="s">
-        <v>87</v>
-      </c>
-      <c r="CA2" t="s">
+      <c r="CB2" t="s">
         <v>151</v>
       </c>
-      <c r="CB2" t="s">
+      <c r="CC2" t="s">
+        <v>87</v>
+      </c>
+      <c r="CD2" t="s">
         <v>152</v>
       </c>
-      <c r="CC2" t="s">
-        <v>87</v>
-      </c>
-      <c r="CD2" t="s">
+      <c r="CE2" t="s">
         <v>153</v>
       </c>
-      <c r="CE2" t="s">
+      <c r="CH2" t="s">
         <v>154</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>155</v>
       </c>
       <c r="CJ2" t="s">
         <v>87</v>
@@ -1653,7 +1650,7 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.15">
       <c r="D3" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="BT3" s="1"/>
       <c r="BU3" s="1"/>
@@ -1665,16 +1662,16 @@
     </row>
     <row r="4" spans="1:97" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" t="s">
         <v>166</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>222</v>
+      </c>
+      <c r="E4" t="s">
         <v>167</v>
-      </c>
-      <c r="D4" t="s">
-        <v>223</v>
-      </c>
-      <c r="E4" t="s">
-        <v>168</v>
       </c>
       <c r="R4" t="s">
         <v>87</v>
@@ -1686,7 +1683,7 @@
         <v>1234</v>
       </c>
       <c r="U4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="V4" t="s">
         <v>87</v>
@@ -1719,16 +1716,16 @@
         <v>94219</v>
       </c>
       <c r="AG4" t="s">
+        <v>169</v>
+      </c>
+      <c r="AH4" t="s">
         <v>170</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ4" t="s">
         <v>171</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>172</v>
       </c>
       <c r="AK4" t="s">
         <v>87</v>
@@ -1755,148 +1752,148 @@
         <v>2130</v>
       </c>
       <c r="AS4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AT4">
         <v>324899</v>
       </c>
       <c r="AU4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AV4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AW4">
         <v>12451324</v>
       </c>
       <c r="AX4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AY4">
         <v>124394</v>
       </c>
       <c r="AZ4" t="s">
+        <v>180</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>177</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BG4" t="s">
         <v>181</v>
       </c>
-      <c r="BE4" t="s">
-        <v>178</v>
-      </c>
-      <c r="BF4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BG4" t="s">
+      <c r="BH4" t="s">
         <v>182</v>
       </c>
-      <c r="BH4" t="s">
-        <v>183</v>
-      </c>
       <c r="BI4" t="s">
         <v>87</v>
       </c>
       <c r="BJ4" t="s">
+        <v>185</v>
+      </c>
+      <c r="BK4" t="s">
         <v>186</v>
       </c>
-      <c r="BK4" t="s">
+      <c r="BL4" t="s">
         <v>187</v>
       </c>
-      <c r="BL4" t="s">
+      <c r="BM4" t="s">
         <v>188</v>
       </c>
-      <c r="BM4" t="s">
+      <c r="BN4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BO4" t="s">
         <v>189</v>
       </c>
-      <c r="BN4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BO4" t="s">
+      <c r="BP4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BQ4" t="s">
         <v>190</v>
       </c>
-      <c r="BP4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BQ4" t="s">
+      <c r="BR4" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BR4" s="1" t="s">
+      <c r="BS4" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="BS4" s="1" t="s">
+      <c r="BT4" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BT4" s="1" t="s">
+      <c r="BU4" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BU4" s="1" t="s">
+      <c r="BV4" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="BV4" s="1" t="s">
+      <c r="BW4" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="BW4" s="1" t="s">
+      <c r="BX4" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="BX4" s="1" t="s">
+      <c r="BY4" t="s">
         <v>198</v>
       </c>
-      <c r="BY4" t="s">
+      <c r="BZ4" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="BZ4" s="1" t="s">
+      <c r="CA4" t="s">
         <v>200</v>
       </c>
-      <c r="CA4" t="s">
+      <c r="CB4" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="CB4" s="1" t="s">
+      <c r="CC4" t="s">
         <v>202</v>
       </c>
-      <c r="CC4" t="s">
+      <c r="CD4" t="s">
         <v>203</v>
       </c>
-      <c r="CD4" t="s">
+      <c r="CE4" t="s">
         <v>204</v>
       </c>
-      <c r="CE4" t="s">
+      <c r="CF4" t="s">
         <v>205</v>
       </c>
-      <c r="CF4" t="s">
+      <c r="CG4" t="s">
         <v>206</v>
       </c>
-      <c r="CG4" t="s">
+      <c r="CH4" t="s">
         <v>207</v>
       </c>
-      <c r="CH4" t="s">
+      <c r="CI4" t="s">
         <v>208</v>
-      </c>
-      <c r="CI4" t="s">
-        <v>209</v>
       </c>
       <c r="CJ4" s="3">
         <v>44124</v>
       </c>
       <c r="CK4" t="s">
+        <v>209</v>
+      </c>
+      <c r="CL4" t="s">
         <v>210</v>
       </c>
-      <c r="CL4" t="s">
+      <c r="CM4" t="s">
         <v>211</v>
       </c>
-      <c r="CM4" t="s">
+      <c r="CN4" t="s">
         <v>212</v>
       </c>
-      <c r="CN4" t="s">
+      <c r="CO4" t="s">
         <v>213</v>
       </c>
-      <c r="CO4" t="s">
+      <c r="CP4" t="s">
         <v>214</v>
       </c>
-      <c r="CP4" t="s">
+      <c r="CQ4" t="s">
         <v>215</v>
       </c>
-      <c r="CQ4" t="s">
-        <v>216</v>
-      </c>
       <c r="CR4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="CS4">
         <v>5.5</v>
@@ -1913,7 +1910,7 @@
         <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E5" t="s">
         <v>97</v>
@@ -1991,14 +1988,14 @@
         <v>100</v>
       </c>
       <c r="AH5" t="s">
+        <v>155</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ5" t="s">
         <v>156</v>
       </c>
-      <c r="AI5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>157</v>
-      </c>
       <c r="AK5" t="s">
         <v>87</v>
       </c>
@@ -2021,7 +2018,7 @@
         <v>87</v>
       </c>
       <c r="AR5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="AS5" t="s">
         <v>88</v>
@@ -2078,7 +2075,7 @@
         <v>87</v>
       </c>
       <c r="BO5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="BP5" t="s">
         <v>87</v>
@@ -2132,25 +2129,25 @@
         <v>123</v>
       </c>
       <c r="CI5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="CJ5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="CK5" t="s">
+        <v>157</v>
+      </c>
+      <c r="CL5" t="s">
         <v>158</v>
       </c>
-      <c r="CL5" t="s">
+      <c r="CM5" t="s">
+        <v>161</v>
+      </c>
+      <c r="CN5" t="s">
+        <v>160</v>
+      </c>
+      <c r="CO5" t="s">
         <v>159</v>
-      </c>
-      <c r="CM5" t="s">
-        <v>162</v>
-      </c>
-      <c r="CN5" t="s">
-        <v>161</v>
-      </c>
-      <c r="CO5" t="s">
-        <v>160</v>
       </c>
       <c r="CP5" t="s">
         <v>125</v>
@@ -2162,7 +2159,7 @@
         <v>123</v>
       </c>
       <c r="CS5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:97" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Identity import; yarn pkg update
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA-ALERT/SaraAlert/test/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aholmes/Developer/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7260ABE2-BDE7-DF47-BF66-000BB3370EDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3857EA3-FB6F-AC43-8F04-70E962BFB615}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="225">
   <si>
     <t>First Name</t>
   </si>
@@ -689,6 +689,12 @@
   </si>
   <si>
     <t>2005-05-42</t>
+  </si>
+  <si>
+    <t>Gender Identity</t>
+  </si>
+  <si>
+    <t>Sexual Orientation</t>
   </si>
 </sst>
 </file>
@@ -1041,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CS12"/>
+  <dimension ref="A1:CU12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="AM1" workbookViewId="0">
-      <selection activeCell="AR6" sqref="AR6"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CL1" workbookViewId="0">
+      <selection activeCell="CT8" sqref="CT8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1148,7 +1154,7 @@
     <col min="97" max="97" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:97" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:99" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1440,8 +1446,14 @@
       <c r="CS1" t="s">
         <v>216</v>
       </c>
+      <c r="CT1" t="s">
+        <v>223</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>224</v>
+      </c>
     </row>
-    <row r="2" spans="1:97" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.15">
       <c r="D2" s="1" t="s">
         <v>220</v>
       </c>
@@ -1648,7 +1660,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:97" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.15">
       <c r="D3" s="1" t="s">
         <v>221</v>
       </c>
@@ -1660,7 +1672,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:97" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>165</v>
       </c>
@@ -1899,7 +1911,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="5" spans="1:97" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:99" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -2162,13 +2174,13 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:97" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:99" x14ac:dyDescent="0.15">
       <c r="BT6" s="1"/>
       <c r="BU6" s="1"/>
       <c r="BW6" s="1"/>
       <c r="CB6" s="1"/>
     </row>
-    <row r="7" spans="1:97" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:99" x14ac:dyDescent="0.15">
       <c r="D7" s="2"/>
       <c r="BL7" s="2"/>
       <c r="BM7" s="2"/>
@@ -2181,7 +2193,7 @@
       <c r="CO7" s="2"/>
       <c r="CP7" s="3"/>
     </row>
-    <row r="8" spans="1:97" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:99" x14ac:dyDescent="0.15">
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -2198,7 +2210,7 @@
       <c r="CB8" s="1"/>
       <c r="CD8" s="1"/>
     </row>
-    <row r="9" spans="1:97" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:99" x14ac:dyDescent="0.15">
       <c r="D9" s="3"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -2215,7 +2227,7 @@
       <c r="CC9" s="1"/>
       <c r="CD9" s="1"/>
     </row>
-    <row r="10" spans="1:97" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:99" x14ac:dyDescent="0.15">
       <c r="AZ10" s="2"/>
       <c r="BE10" s="2"/>
       <c r="BO10" s="3"/>
@@ -2224,7 +2236,7 @@
       <c r="CO10" s="3"/>
       <c r="CP10" s="2"/>
     </row>
-    <row r="12" spans="1:97" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:99" x14ac:dyDescent="0.15">
       <c r="D12" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
validate phone numbers for import and exports
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aholmes/Developer/SaraAlert/test/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA-ALERT/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3857EA3-FB6F-AC43-8F04-70E962BFB615}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BEAD7B-BECB-CD41-A42A-9EB2C7739FC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="225">
   <si>
     <t>First Name</t>
   </si>
@@ -538,9 +538,6 @@
     <t>$@)!(@</t>
   </si>
   <si>
-    <t>ABC</t>
-  </si>
-  <si>
     <t>ZYX</t>
   </si>
   <si>
@@ -695,6 +692,9 @@
   </si>
   <si>
     <t>Sexual Orientation</t>
+  </si>
+  <si>
+    <t>333-333-3333</t>
   </si>
 </sst>
 </file>
@@ -1049,8 +1049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CU12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CL1" workbookViewId="0">
-      <selection activeCell="CT8" sqref="CT8"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="AU6" sqref="AU6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1441,21 +1441,21 @@
         <v>122</v>
       </c>
       <c r="CR1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="CS1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="CT1" t="s">
+        <v>222</v>
+      </c>
+      <c r="CU1" t="s">
         <v>223</v>
-      </c>
-      <c r="CU1" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:99" x14ac:dyDescent="0.15">
       <c r="D2" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" t="s">
         <v>125</v>
@@ -1548,7 +1548,7 @@
         <v>138</v>
       </c>
       <c r="AV2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AW2" t="s">
         <v>139</v>
@@ -1557,22 +1557,22 @@
         <v>140</v>
       </c>
       <c r="AZ2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BE2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="BF2" t="s">
         <v>87</v>
       </c>
       <c r="BG2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="BH2" t="s">
         <v>87</v>
       </c>
       <c r="BI2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="BJ2" t="s">
         <v>87</v>
@@ -1662,7 +1662,7 @@
     </row>
     <row r="3" spans="1:99" x14ac:dyDescent="0.15">
       <c r="D3" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="BT3" s="1"/>
       <c r="BU3" s="1"/>
@@ -1680,7 +1680,7 @@
         <v>166</v>
       </c>
       <c r="D4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E4" t="s">
         <v>167</v>
@@ -1763,149 +1763,149 @@
       <c r="AR4">
         <v>2130</v>
       </c>
-      <c r="AS4" t="s">
-        <v>172</v>
+      <c r="AS4">
+        <v>12345</v>
       </c>
       <c r="AT4">
         <v>324899</v>
       </c>
       <c r="AU4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AV4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AW4">
         <v>12451324</v>
       </c>
       <c r="AX4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AY4">
         <v>124394</v>
       </c>
       <c r="AZ4" t="s">
+        <v>179</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>176</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BG4" t="s">
         <v>180</v>
       </c>
-      <c r="BE4" t="s">
-        <v>177</v>
-      </c>
-      <c r="BF4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BG4" t="s">
+      <c r="BH4" t="s">
         <v>181</v>
       </c>
-      <c r="BH4" t="s">
-        <v>182</v>
-      </c>
       <c r="BI4" t="s">
         <v>87</v>
       </c>
       <c r="BJ4" t="s">
+        <v>184</v>
+      </c>
+      <c r="BK4" t="s">
         <v>185</v>
       </c>
-      <c r="BK4" t="s">
+      <c r="BL4" t="s">
         <v>186</v>
       </c>
-      <c r="BL4" t="s">
+      <c r="BM4" t="s">
         <v>187</v>
       </c>
-      <c r="BM4" t="s">
+      <c r="BN4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BO4" t="s">
         <v>188</v>
       </c>
-      <c r="BN4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BO4" t="s">
+      <c r="BP4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BQ4" t="s">
         <v>189</v>
       </c>
-      <c r="BP4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BQ4" t="s">
+      <c r="BR4" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BR4" s="1" t="s">
+      <c r="BS4" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BS4" s="1" t="s">
+      <c r="BT4" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="BT4" s="1" t="s">
+      <c r="BU4" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BU4" s="1" t="s">
+      <c r="BV4" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BV4" s="1" t="s">
+      <c r="BW4" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="BW4" s="1" t="s">
+      <c r="BX4" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="BX4" s="1" t="s">
+      <c r="BY4" t="s">
         <v>197</v>
       </c>
-      <c r="BY4" t="s">
+      <c r="BZ4" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="BZ4" s="1" t="s">
+      <c r="CA4" t="s">
         <v>199</v>
       </c>
-      <c r="CA4" t="s">
+      <c r="CB4" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="CB4" s="1" t="s">
+      <c r="CC4" t="s">
         <v>201</v>
       </c>
-      <c r="CC4" t="s">
+      <c r="CD4" t="s">
         <v>202</v>
       </c>
-      <c r="CD4" t="s">
+      <c r="CE4" t="s">
         <v>203</v>
       </c>
-      <c r="CE4" t="s">
+      <c r="CF4" t="s">
         <v>204</v>
       </c>
-      <c r="CF4" t="s">
+      <c r="CG4" t="s">
         <v>205</v>
       </c>
-      <c r="CG4" t="s">
+      <c r="CH4" t="s">
         <v>206</v>
       </c>
-      <c r="CH4" t="s">
+      <c r="CI4" t="s">
         <v>207</v>
-      </c>
-      <c r="CI4" t="s">
-        <v>208</v>
       </c>
       <c r="CJ4" s="3">
         <v>44124</v>
       </c>
       <c r="CK4" t="s">
+        <v>208</v>
+      </c>
+      <c r="CL4" t="s">
         <v>209</v>
       </c>
-      <c r="CL4" t="s">
+      <c r="CM4" t="s">
         <v>210</v>
       </c>
-      <c r="CM4" t="s">
+      <c r="CN4" t="s">
         <v>211</v>
       </c>
-      <c r="CN4" t="s">
+      <c r="CO4" t="s">
         <v>212</v>
       </c>
-      <c r="CO4" t="s">
+      <c r="CP4" t="s">
         <v>213</v>
       </c>
-      <c r="CP4" t="s">
+      <c r="CQ4" t="s">
         <v>214</v>
       </c>
-      <c r="CQ4" t="s">
-        <v>215</v>
-      </c>
       <c r="CR4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="CS4">
         <v>5.5</v>
@@ -1922,7 +1922,7 @@
         <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E5" t="s">
         <v>97</v>
@@ -2039,7 +2039,7 @@
         <v>89</v>
       </c>
       <c r="AU5" t="s">
-        <v>88</v>
+        <v>224</v>
       </c>
       <c r="AV5" t="s">
         <v>90</v>

</xml_diff>

<commit_message>
fixed most of the test issues, I think there's another hardcoded index I missed
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA-ALERT/SaraAlert/test/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashankland/git/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BEAD7B-BECB-CD41-A42A-9EB2C7739FC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2EEC82-0BEA-544F-B0D7-02E90DA6A7BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitorees" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="228">
   <si>
     <t>First Name</t>
   </si>
@@ -695,6 +695,15 @@
   </si>
   <si>
     <t>333-333-3333</t>
+  </si>
+  <si>
+    <t>Race Unknown</t>
+  </si>
+  <si>
+    <t>Race Other</t>
+  </si>
+  <si>
+    <t>Race Refused to Answer</t>
   </si>
 </sst>
 </file>
@@ -1047,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CU12"/>
+  <dimension ref="A1:CX12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="AU6" sqref="AU6"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1065,96 +1074,97 @@
     <col min="8" max="8" width="28.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="22" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="35" customWidth="1"/>
+    <col min="14" max="14" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.5" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="29" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="29" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="30" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="24" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="15" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="20" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="38.83203125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="30" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="24" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="32.83203125" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="35.1640625" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="38" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="12" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="16" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="12" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="29" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="30" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="24" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="15" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="20" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="30" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="24" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="38" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="12" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="16" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="12" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1186,274 +1196,283 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>225</v>
+      </c>
+      <c r="L1" t="s">
+        <v>226</v>
+      </c>
+      <c r="M1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AN1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AO1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AP1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AQ1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AR1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AS1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AT1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AU1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AV1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AW1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AX1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AY1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AZ1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BA1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BB1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BC1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BD1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BE1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BF1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BG1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BH1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BI1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BJ1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BK1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BL1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BM1" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BN1" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BO1" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BP1" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BQ1" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BR1" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BS1" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BT1" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BW1" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BX1" t="s">
         <v>72</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BY1" t="s">
         <v>73</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BZ1" t="s">
         <v>74</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="CA1" t="s">
         <v>75</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="CB1" t="s">
         <v>76</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CC1" t="s">
         <v>77</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CD1" t="s">
         <v>78</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CE1" t="s">
         <v>79</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CF1" t="s">
         <v>80</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CG1" t="s">
         <v>81</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CH1" t="s">
         <v>82</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CI1" t="s">
         <v>83</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CJ1" t="s">
         <v>84</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CK1" t="s">
         <v>113</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CL1" t="s">
         <v>114</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CM1" t="s">
         <v>115</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CN1" t="s">
         <v>116</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CO1" t="s">
         <v>117</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CP1" t="s">
         <v>118</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CQ1" t="s">
         <v>119</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="CR1" t="s">
         <v>120</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="CS1" t="s">
         <v>121</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="CT1" t="s">
         <v>122</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="CU1" t="s">
         <v>217</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="CV1" t="s">
         <v>215</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="CW1" t="s">
         <v>222</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="CX1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:102" x14ac:dyDescent="0.15">
       <c r="D2" s="1" t="s">
         <v>219</v>
       </c>
@@ -1475,28 +1494,19 @@
       <c r="J2" t="s">
         <v>131</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>132</v>
       </c>
-      <c r="M2" t="s">
-        <v>87</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q2" t="s">
         <v>134</v>
       </c>
-      <c r="O2" t="s">
-        <v>87</v>
-      </c>
       <c r="R2" t="s">
         <v>87</v>
       </c>
-      <c r="X2" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z2" t="s">
+      <c r="U2" t="s">
         <v>87</v>
       </c>
       <c r="AA2" t="s">
@@ -1514,13 +1524,13 @@
       <c r="AE2" t="s">
         <v>87</v>
       </c>
-      <c r="AK2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM2" t="s">
+      <c r="AF2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH2" t="s">
         <v>87</v>
       </c>
       <c r="AN2" t="s">
@@ -1536,143 +1546,152 @@
         <v>87</v>
       </c>
       <c r="AR2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AU2" t="s">
         <v>135</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AV2" t="s">
         <v>136</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AW2" t="s">
         <v>137</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AX2" t="s">
         <v>138</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AY2" t="s">
         <v>173</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AZ2" t="s">
         <v>139</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="BA2" t="s">
         <v>140</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="BC2" t="s">
         <v>178</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BH2" t="s">
         <v>177</v>
       </c>
-      <c r="BF2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BG2" t="s">
+      <c r="BI2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BJ2" t="s">
         <v>183</v>
       </c>
-      <c r="BH2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BI2" t="s">
+      <c r="BK2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BL2" t="s">
         <v>182</v>
       </c>
-      <c r="BJ2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BL2" t="s">
+      <c r="BM2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BO2" t="s">
         <v>141</v>
       </c>
-      <c r="BM2" t="s">
+      <c r="BP2" t="s">
         <v>142</v>
       </c>
-      <c r="BN2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BO2" s="2"/>
-      <c r="BP2" t="s">
+      <c r="BQ2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BR2" s="2"/>
+      <c r="BS2" t="s">
         <v>92</v>
       </c>
-      <c r="BQ2" t="s">
+      <c r="BT2" t="s">
         <v>93</v>
       </c>
-      <c r="BR2" s="1" t="s">
+      <c r="BU2" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="BS2" s="1" t="s">
+      <c r="BV2" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="BT2" t="s">
+      <c r="BW2" t="s">
         <v>146</v>
       </c>
-      <c r="BU2" t="s">
+      <c r="BX2" t="s">
         <v>147</v>
       </c>
-      <c r="BV2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BW2" t="s">
+      <c r="BY2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BZ2" t="s">
         <v>148</v>
       </c>
-      <c r="BX2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BY2" t="s">
+      <c r="CA2" t="s">
+        <v>87</v>
+      </c>
+      <c r="CB2" t="s">
         <v>149</v>
       </c>
-      <c r="BZ2" t="s">
-        <v>87</v>
-      </c>
-      <c r="CA2" t="s">
+      <c r="CC2" t="s">
+        <v>87</v>
+      </c>
+      <c r="CD2" t="s">
         <v>150</v>
       </c>
-      <c r="CB2" t="s">
+      <c r="CE2" t="s">
         <v>151</v>
       </c>
-      <c r="CC2" t="s">
-        <v>87</v>
-      </c>
-      <c r="CD2" t="s">
+      <c r="CF2" t="s">
+        <v>87</v>
+      </c>
+      <c r="CG2" t="s">
         <v>152</v>
       </c>
-      <c r="CE2" t="s">
+      <c r="CH2" t="s">
         <v>153</v>
       </c>
-      <c r="CH2" t="s">
+      <c r="CK2" t="s">
         <v>154</v>
       </c>
-      <c r="CJ2" t="s">
-        <v>87</v>
-      </c>
       <c r="CM2" t="s">
         <v>87</v>
       </c>
-      <c r="CN2" t="s">
+      <c r="CP2" t="s">
         <v>87</v>
       </c>
       <c r="CQ2" t="s">
         <v>87</v>
       </c>
-      <c r="CR2" t="s">
+      <c r="CT2" t="s">
+        <v>87</v>
+      </c>
+      <c r="CU2" t="s">
         <v>125</v>
       </c>
-      <c r="CS2">
+      <c r="CV2">
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:102" x14ac:dyDescent="0.15">
       <c r="D3" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="BT3" s="1"/>
-      <c r="BU3" s="1"/>
       <c r="BW3" s="1"/>
-      <c r="CB3" s="1"/>
-      <c r="CR3" t="s">
+      <c r="BX3" s="1"/>
+      <c r="BZ3" s="1"/>
+      <c r="CE3" s="1"/>
+      <c r="CU3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>165</v>
       </c>
@@ -1685,36 +1704,27 @@
       <c r="E4" t="s">
         <v>167</v>
       </c>
-      <c r="R4" t="s">
-        <v>87</v>
-      </c>
-      <c r="S4">
+      <c r="U4" t="s">
+        <v>87</v>
+      </c>
+      <c r="V4">
         <v>887</v>
       </c>
-      <c r="T4">
+      <c r="W4">
         <v>1234</v>
       </c>
-      <c r="U4" t="s">
+      <c r="X4" t="s">
         <v>168</v>
       </c>
-      <c r="V4" t="s">
-        <v>87</v>
-      </c>
-      <c r="W4">
+      <c r="Y4" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z4">
         <v>381942349</v>
       </c>
-      <c r="X4">
+      <c r="AA4">
         <v>123</v>
       </c>
-      <c r="Z4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>87</v>
-      </c>
       <c r="AC4" t="s">
         <v>87</v>
       </c>
@@ -1724,30 +1734,30 @@
       <c r="AE4" t="s">
         <v>87</v>
       </c>
-      <c r="AF4">
+      <c r="AF4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI4">
         <v>94219</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AJ4" t="s">
         <v>169</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AK4" t="s">
         <v>170</v>
       </c>
-      <c r="AI4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ4" t="s">
+      <c r="AL4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM4" t="s">
         <v>171</v>
       </c>
-      <c r="AK4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>87</v>
-      </c>
       <c r="AN4" t="s">
         <v>87</v>
       </c>
@@ -1760,158 +1770,167 @@
       <c r="AQ4" t="s">
         <v>87</v>
       </c>
-      <c r="AR4">
+      <c r="AR4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AU4">
         <v>2130</v>
       </c>
-      <c r="AS4">
+      <c r="AV4">
         <v>12345</v>
       </c>
-      <c r="AT4">
+      <c r="AW4">
         <v>324899</v>
       </c>
-      <c r="AU4" t="s">
+      <c r="AX4" t="s">
         <v>172</v>
       </c>
-      <c r="AV4" t="s">
+      <c r="AY4" t="s">
         <v>174</v>
       </c>
-      <c r="AW4">
+      <c r="AZ4">
         <v>12451324</v>
       </c>
-      <c r="AX4" t="s">
+      <c r="BA4" t="s">
         <v>175</v>
       </c>
-      <c r="AY4">
+      <c r="BB4">
         <v>124394</v>
       </c>
-      <c r="AZ4" t="s">
+      <c r="BC4" t="s">
         <v>179</v>
       </c>
-      <c r="BE4" t="s">
+      <c r="BH4" t="s">
         <v>176</v>
       </c>
-      <c r="BF4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BG4" t="s">
+      <c r="BI4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BJ4" t="s">
         <v>180</v>
       </c>
-      <c r="BH4" t="s">
+      <c r="BK4" t="s">
         <v>181</v>
       </c>
-      <c r="BI4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BJ4" t="s">
+      <c r="BL4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BM4" t="s">
         <v>184</v>
       </c>
-      <c r="BK4" t="s">
+      <c r="BN4" t="s">
         <v>185</v>
       </c>
-      <c r="BL4" t="s">
+      <c r="BO4" t="s">
         <v>186</v>
       </c>
-      <c r="BM4" t="s">
+      <c r="BP4" t="s">
         <v>187</v>
       </c>
-      <c r="BN4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BO4" t="s">
+      <c r="BQ4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BR4" t="s">
         <v>188</v>
       </c>
-      <c r="BP4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BQ4" t="s">
+      <c r="BS4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BT4" t="s">
         <v>189</v>
       </c>
-      <c r="BR4" s="1" t="s">
+      <c r="BU4" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BS4" s="1" t="s">
+      <c r="BV4" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BT4" s="1" t="s">
+      <c r="BW4" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="BU4" s="1" t="s">
+      <c r="BX4" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BV4" s="1" t="s">
+      <c r="BY4" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BW4" s="1" t="s">
+      <c r="BZ4" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="BX4" s="1" t="s">
+      <c r="CA4" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="BY4" t="s">
+      <c r="CB4" t="s">
         <v>197</v>
       </c>
-      <c r="BZ4" s="1" t="s">
+      <c r="CC4" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="CA4" t="s">
+      <c r="CD4" t="s">
         <v>199</v>
       </c>
-      <c r="CB4" s="1" t="s">
+      <c r="CE4" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="CC4" t="s">
+      <c r="CF4" t="s">
         <v>201</v>
       </c>
-      <c r="CD4" t="s">
+      <c r="CG4" t="s">
         <v>202</v>
       </c>
-      <c r="CE4" t="s">
+      <c r="CH4" t="s">
         <v>203</v>
       </c>
-      <c r="CF4" t="s">
+      <c r="CI4" t="s">
         <v>204</v>
       </c>
-      <c r="CG4" t="s">
+      <c r="CJ4" t="s">
         <v>205</v>
       </c>
-      <c r="CH4" t="s">
+      <c r="CK4" t="s">
         <v>206</v>
       </c>
-      <c r="CI4" t="s">
+      <c r="CL4" t="s">
         <v>207</v>
       </c>
-      <c r="CJ4" s="3">
+      <c r="CM4" s="3">
         <v>44124</v>
       </c>
-      <c r="CK4" t="s">
+      <c r="CN4" t="s">
         <v>208</v>
       </c>
-      <c r="CL4" t="s">
+      <c r="CO4" t="s">
         <v>209</v>
       </c>
-      <c r="CM4" t="s">
+      <c r="CP4" t="s">
         <v>210</v>
       </c>
-      <c r="CN4" t="s">
+      <c r="CQ4" t="s">
         <v>211</v>
       </c>
-      <c r="CO4" t="s">
+      <c r="CR4" t="s">
         <v>212</v>
       </c>
-      <c r="CP4" t="s">
+      <c r="CS4" t="s">
         <v>213</v>
       </c>
-      <c r="CQ4" t="s">
+      <c r="CT4" t="s">
         <v>214</v>
       </c>
-      <c r="CR4" t="s">
+      <c r="CU4" t="s">
         <v>218</v>
       </c>
-      <c r="CS4">
+      <c r="CV4">
         <v>5.5</v>
       </c>
     </row>
-    <row r="5" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -1942,48 +1961,39 @@
       <c r="J5" t="s">
         <v>85</v>
       </c>
-      <c r="K5" t="s">
+      <c r="N5" t="s">
         <v>98</v>
       </c>
-      <c r="M5" t="s">
-        <v>87</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="P5" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q5" t="s">
         <v>85</v>
       </c>
-      <c r="O5" t="s">
-        <v>87</v>
-      </c>
       <c r="R5" t="s">
         <v>87</v>
       </c>
-      <c r="S5" t="s">
+      <c r="U5" t="s">
+        <v>87</v>
+      </c>
+      <c r="V5" t="s">
         <v>99</v>
       </c>
-      <c r="T5" t="s">
+      <c r="W5" t="s">
         <v>100</v>
       </c>
-      <c r="U5" t="s">
+      <c r="X5" t="s">
         <v>125</v>
       </c>
-      <c r="V5" t="s">
-        <v>87</v>
-      </c>
-      <c r="W5" t="s">
+      <c r="Y5" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z5" t="s">
         <v>101</v>
       </c>
-      <c r="X5" t="s">
+      <c r="AA5" t="s">
         <v>128</v>
       </c>
-      <c r="Z5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>87</v>
-      </c>
       <c r="AC5" t="s">
         <v>87</v>
       </c>
@@ -1994,29 +2004,29 @@
         <v>87</v>
       </c>
       <c r="AF5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI5" t="s">
         <v>99</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AJ5" t="s">
         <v>100</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AK5" t="s">
         <v>155</v>
       </c>
-      <c r="AI5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ5" t="s">
+      <c r="AL5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM5" t="s">
         <v>156</v>
       </c>
-      <c r="AK5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>87</v>
-      </c>
       <c r="AN5" t="s">
         <v>87</v>
       </c>
@@ -2030,213 +2040,228 @@
         <v>87</v>
       </c>
       <c r="AR5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AU5" t="s">
         <v>125</v>
       </c>
-      <c r="AS5" t="s">
+      <c r="AV5" t="s">
         <v>88</v>
       </c>
-      <c r="AT5" t="s">
+      <c r="AW5" t="s">
         <v>89</v>
       </c>
-      <c r="AU5" t="s">
+      <c r="AX5" t="s">
         <v>224</v>
       </c>
-      <c r="AV5" t="s">
+      <c r="AY5" t="s">
         <v>90</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="AZ5" t="s">
         <v>127</v>
       </c>
-      <c r="AX5" t="s">
+      <c r="BA5" t="s">
         <v>102</v>
       </c>
-      <c r="AY5" t="s">
+      <c r="BB5" t="s">
         <v>103</v>
       </c>
-      <c r="AZ5" t="s">
+      <c r="BC5" t="s">
         <v>91</v>
       </c>
-      <c r="BE5" t="s">
+      <c r="BH5" t="s">
         <v>91</v>
       </c>
-      <c r="BF5" t="s">
-        <v>87</v>
-      </c>
-      <c r="BG5" t="s">
+      <c r="BI5" t="s">
+        <v>87</v>
+      </c>
+      <c r="BJ5" t="s">
         <v>104</v>
       </c>
-      <c r="BH5" t="s">
+      <c r="BK5" t="s">
         <v>105</v>
       </c>
-      <c r="BI5" t="s">
-        <v>87</v>
-      </c>
-      <c r="BJ5" t="s">
+      <c r="BL5" t="s">
+        <v>87</v>
+      </c>
+      <c r="BM5" t="s">
         <v>106</v>
       </c>
-      <c r="BK5" t="s">
+      <c r="BN5" t="s">
         <v>107</v>
       </c>
-      <c r="BL5" t="s">
+      <c r="BO5" t="s">
         <v>108</v>
       </c>
-      <c r="BM5" t="s">
+      <c r="BP5" t="s">
         <v>109</v>
       </c>
-      <c r="BN5" t="s">
-        <v>87</v>
-      </c>
-      <c r="BO5" t="s">
+      <c r="BQ5" t="s">
+        <v>87</v>
+      </c>
+      <c r="BR5" t="s">
         <v>143</v>
       </c>
-      <c r="BP5" t="s">
-        <v>87</v>
-      </c>
-      <c r="BQ5" t="s">
+      <c r="BS5" t="s">
+        <v>87</v>
+      </c>
+      <c r="BT5" t="s">
         <v>110</v>
       </c>
-      <c r="BR5" s="1" t="s">
+      <c r="BU5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="BS5" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="BT5" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="BU5" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="BV5" t="s">
+      <c r="BV5" s="1" t="s">
         <v>87</v>
       </c>
       <c r="BW5" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="BX5" t="s">
-        <v>87</v>
+      <c r="BX5" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="BY5" t="s">
+        <v>87</v>
+      </c>
+      <c r="BZ5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="CA5" t="s">
+        <v>87</v>
+      </c>
+      <c r="CB5" t="s">
         <v>85</v>
       </c>
-      <c r="BZ5" t="s">
-        <v>87</v>
-      </c>
-      <c r="CA5" t="s">
+      <c r="CC5" t="s">
+        <v>87</v>
+      </c>
+      <c r="CD5" t="s">
         <v>85</v>
       </c>
-      <c r="CB5" s="1" t="s">
+      <c r="CE5" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="CC5" t="s">
-        <v>87</v>
-      </c>
-      <c r="CD5" t="s">
+      <c r="CF5" t="s">
+        <v>87</v>
+      </c>
+      <c r="CG5" t="s">
         <v>111</v>
       </c>
-      <c r="CE5" t="s">
+      <c r="CH5" t="s">
         <v>112</v>
       </c>
-      <c r="CH5" t="s">
+      <c r="CK5" t="s">
         <v>123</v>
       </c>
-      <c r="CI5" t="s">
+      <c r="CL5" t="s">
         <v>163</v>
       </c>
-      <c r="CJ5" t="s">
+      <c r="CM5" t="s">
         <v>162</v>
       </c>
-      <c r="CK5" t="s">
+      <c r="CN5" t="s">
         <v>157</v>
       </c>
-      <c r="CL5" t="s">
+      <c r="CO5" t="s">
         <v>158</v>
       </c>
-      <c r="CM5" t="s">
+      <c r="CP5" t="s">
         <v>161</v>
       </c>
-      <c r="CN5" t="s">
+      <c r="CQ5" t="s">
         <v>160</v>
       </c>
-      <c r="CO5" t="s">
+      <c r="CR5" t="s">
         <v>159</v>
       </c>
-      <c r="CP5" t="s">
+      <c r="CS5" t="s">
         <v>125</v>
       </c>
-      <c r="CQ5" t="s">
+      <c r="CT5" t="s">
         <v>126</v>
       </c>
-      <c r="CR5">
+      <c r="CU5">
         <v>123</v>
       </c>
-      <c r="CS5" t="s">
+      <c r="CV5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:99" x14ac:dyDescent="0.15">
-      <c r="BT6" s="1"/>
-      <c r="BU6" s="1"/>
+    <row r="6" spans="1:102" x14ac:dyDescent="0.15">
       <c r="BW6" s="1"/>
-      <c r="CB6" s="1"/>
+      <c r="BX6" s="1"/>
+      <c r="BZ6" s="1"/>
+      <c r="CE6" s="1"/>
     </row>
-    <row r="7" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:102" x14ac:dyDescent="0.15">
       <c r="D7" s="2"/>
-      <c r="BL7" s="2"/>
-      <c r="BM7" s="2"/>
       <c r="BO7" s="2"/>
-      <c r="BT7" s="1"/>
-      <c r="BU7" s="1"/>
+      <c r="BP7" s="2"/>
+      <c r="BR7" s="2"/>
       <c r="BW7" s="1"/>
-      <c r="CB7" s="1"/>
-      <c r="CH7" s="3"/>
-      <c r="CO7" s="2"/>
-      <c r="CP7" s="3"/>
+      <c r="BX7" s="1"/>
+      <c r="BZ7" s="1"/>
+      <c r="CE7" s="1"/>
+      <c r="CK7" s="3"/>
+      <c r="CR7" s="2"/>
+      <c r="CS7" s="3"/>
     </row>
-    <row r="8" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:102" x14ac:dyDescent="0.15">
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="BR8"/>
-      <c r="BT8" s="1"/>
-      <c r="BU8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="BU8"/>
       <c r="BW8" s="1"/>
       <c r="BX8" s="1"/>
-      <c r="BY8" s="1"/>
+      <c r="BZ8" s="1"/>
       <c r="CA8" s="1"/>
       <c r="CB8" s="1"/>
       <c r="CD8" s="1"/>
+      <c r="CE8" s="1"/>
+      <c r="CG8" s="1"/>
     </row>
-    <row r="9" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:102" x14ac:dyDescent="0.15">
       <c r="D9" s="3"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="AZ9" s="3"/>
-      <c r="BE9" s="3"/>
-      <c r="BR9"/>
-      <c r="BY9" s="1"/>
-      <c r="CA9" s="1"/>
-      <c r="CC9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="BC9" s="3"/>
+      <c r="BH9" s="3"/>
+      <c r="BU9"/>
+      <c r="CB9" s="1"/>
       <c r="CD9" s="1"/>
+      <c r="CF9" s="1"/>
+      <c r="CG9" s="1"/>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.15">
-      <c r="AZ10" s="2"/>
-      <c r="BE10" s="2"/>
-      <c r="BO10" s="3"/>
-      <c r="CK10" s="3"/>
-      <c r="CL10" s="2"/>
-      <c r="CO10" s="3"/>
-      <c r="CP10" s="2"/>
+    <row r="10" spans="1:102" x14ac:dyDescent="0.15">
+      <c r="BC10" s="2"/>
+      <c r="BH10" s="2"/>
+      <c r="BR10" s="3"/>
+      <c r="CN10" s="3"/>
+      <c r="CO10" s="2"/>
+      <c r="CR10" s="3"/>
+      <c r="CS10" s="2"/>
     </row>
-    <row r="12" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:102" x14ac:dyDescent="0.15">
       <c r="D12" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
redid tables to have new fields at the end, ready for push?
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashankland/git/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2EEC82-0BEA-544F-B0D7-02E90DA6A7BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682A9255-6649-804C-BF9E-56F81E708E90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1058,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CX12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CL1" workbookViewId="0">
+      <selection activeCell="CX1" sqref="CX1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1074,94 +1074,98 @@
     <col min="8" max="8" width="28.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="35" customWidth="1"/>
-    <col min="14" max="14" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21.5" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="29" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="29" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="29" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="30" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="24" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="15" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="20" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="38.83203125" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="30" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="24" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="32.83203125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="35.1640625" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="38" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="12" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="16" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="12" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="30" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="24" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="20" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="30" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="24" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="38" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="12" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="16" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="12" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="17.33203125" customWidth="1"/>
+    <col min="99" max="99" width="26.33203125" customWidth="1"/>
+    <col min="100" max="100" width="17.1640625" customWidth="1"/>
+    <col min="101" max="101" width="17.6640625" customWidth="1"/>
+    <col min="102" max="102" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:102" x14ac:dyDescent="0.15">
@@ -1196,280 +1200,280 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>77</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>79</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>80</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>81</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>82</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>83</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>84</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>113</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>114</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>115</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>116</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>117</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>118</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>119</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>120</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>121</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>122</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>217</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>215</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>222</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>223</v>
+      </c>
+      <c r="CV1" t="s">
         <v>225</v>
       </c>
-      <c r="L1" t="s">
+      <c r="CW1" t="s">
         <v>226</v>
       </c>
-      <c r="M1" t="s">
+      <c r="CX1" t="s">
         <v>227</v>
-      </c>
-      <c r="N1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" t="s">
-        <v>18</v>
-      </c>
-      <c r="W1" t="s">
-        <v>19</v>
-      </c>
-      <c r="X1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>48</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>49</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>57</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>66</v>
-      </c>
-      <c r="BS1" t="s">
-        <v>67</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>68</v>
-      </c>
-      <c r="BU1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BV1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="BW1" t="s">
-        <v>71</v>
-      </c>
-      <c r="BX1" t="s">
-        <v>72</v>
-      </c>
-      <c r="BY1" t="s">
-        <v>73</v>
-      </c>
-      <c r="BZ1" t="s">
-        <v>74</v>
-      </c>
-      <c r="CA1" t="s">
-        <v>75</v>
-      </c>
-      <c r="CB1" t="s">
-        <v>76</v>
-      </c>
-      <c r="CC1" t="s">
-        <v>77</v>
-      </c>
-      <c r="CD1" t="s">
-        <v>78</v>
-      </c>
-      <c r="CE1" t="s">
-        <v>79</v>
-      </c>
-      <c r="CF1" t="s">
-        <v>80</v>
-      </c>
-      <c r="CG1" t="s">
-        <v>81</v>
-      </c>
-      <c r="CH1" t="s">
-        <v>82</v>
-      </c>
-      <c r="CI1" t="s">
-        <v>83</v>
-      </c>
-      <c r="CJ1" t="s">
-        <v>84</v>
-      </c>
-      <c r="CK1" t="s">
-        <v>113</v>
-      </c>
-      <c r="CL1" t="s">
-        <v>114</v>
-      </c>
-      <c r="CM1" t="s">
-        <v>115</v>
-      </c>
-      <c r="CN1" t="s">
-        <v>116</v>
-      </c>
-      <c r="CO1" t="s">
-        <v>117</v>
-      </c>
-      <c r="CP1" t="s">
-        <v>118</v>
-      </c>
-      <c r="CQ1" t="s">
-        <v>119</v>
-      </c>
-      <c r="CR1" t="s">
-        <v>120</v>
-      </c>
-      <c r="CS1" t="s">
-        <v>121</v>
-      </c>
-      <c r="CT1" t="s">
-        <v>122</v>
-      </c>
-      <c r="CU1" t="s">
-        <v>217</v>
-      </c>
-      <c r="CV1" t="s">
-        <v>215</v>
-      </c>
-      <c r="CW1" t="s">
-        <v>222</v>
-      </c>
-      <c r="CX1" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:102" x14ac:dyDescent="0.15">
@@ -1494,19 +1498,28 @@
       <c r="J2" t="s">
         <v>131</v>
       </c>
+      <c r="K2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M2" t="s">
+        <v>87</v>
+      </c>
       <c r="N2" t="s">
-        <v>132</v>
-      </c>
-      <c r="P2" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q2" t="s">
         <v>134</v>
       </c>
+      <c r="O2" t="s">
+        <v>87</v>
+      </c>
       <c r="R2" t="s">
         <v>87</v>
       </c>
-      <c r="U2" t="s">
+      <c r="X2" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z2" t="s">
         <v>87</v>
       </c>
       <c r="AA2" t="s">
@@ -1524,13 +1537,13 @@
       <c r="AE2" t="s">
         <v>87</v>
       </c>
-      <c r="AF2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AH2" t="s">
+      <c r="AK2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM2" t="s">
         <v>87</v>
       </c>
       <c r="AN2" t="s">
@@ -1546,136 +1559,127 @@
         <v>87</v>
       </c>
       <c r="AR2" t="s">
-        <v>87</v>
+        <v>135</v>
       </c>
       <c r="AS2" t="s">
-        <v>87</v>
+        <v>136</v>
       </c>
       <c r="AT2" t="s">
-        <v>87</v>
+        <v>137</v>
       </c>
       <c r="AU2" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="AV2" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="AW2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AX2" t="s">
-        <v>138</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>173</v>
+        <v>140</v>
       </c>
       <c r="AZ2" t="s">
-        <v>139</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>140</v>
-      </c>
-      <c r="BC2" t="s">
         <v>178</v>
       </c>
+      <c r="BE2" t="s">
+        <v>177</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>183</v>
+      </c>
       <c r="BH2" t="s">
-        <v>177</v>
+        <v>87</v>
       </c>
       <c r="BI2" t="s">
-        <v>87</v>
+        <v>182</v>
       </c>
       <c r="BJ2" t="s">
-        <v>183</v>
+        <v>87</v>
       </c>
       <c r="BK2" t="s">
         <v>87</v>
       </c>
       <c r="BL2" t="s">
-        <v>182</v>
+        <v>141</v>
       </c>
       <c r="BM2" t="s">
-        <v>87</v>
+        <v>142</v>
       </c>
       <c r="BN2" t="s">
         <v>87</v>
       </c>
-      <c r="BO2" t="s">
-        <v>141</v>
-      </c>
+      <c r="BO2" s="2"/>
       <c r="BP2" t="s">
-        <v>142</v>
+        <v>92</v>
       </c>
       <c r="BQ2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BR2" s="2"/>
-      <c r="BS2" t="s">
-        <v>92</v>
+        <v>93</v>
+      </c>
+      <c r="BR2" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="BS2" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="BT2" t="s">
-        <v>93</v>
-      </c>
-      <c r="BU2" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="BV2" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>147</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>87</v>
       </c>
       <c r="BW2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="BX2" t="s">
-        <v>147</v>
+        <v>87</v>
       </c>
       <c r="BY2" t="s">
-        <v>87</v>
+        <v>149</v>
       </c>
       <c r="BZ2" t="s">
-        <v>148</v>
+        <v>87</v>
       </c>
       <c r="CA2" t="s">
-        <v>87</v>
+        <v>150</v>
       </c>
       <c r="CB2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="CC2" t="s">
         <v>87</v>
       </c>
       <c r="CD2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="CE2" t="s">
-        <v>151</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>87</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="CH2" t="s">
-        <v>153</v>
-      </c>
-      <c r="CK2" t="s">
         <v>154</v>
       </c>
+      <c r="CJ2" t="s">
+        <v>87</v>
+      </c>
       <c r="CM2" t="s">
         <v>87</v>
       </c>
-      <c r="CP2" t="s">
+      <c r="CN2" t="s">
         <v>87</v>
       </c>
       <c r="CQ2" t="s">
         <v>87</v>
       </c>
-      <c r="CT2" t="s">
-        <v>87</v>
-      </c>
-      <c r="CU2" t="s">
+      <c r="CR2" t="s">
         <v>125</v>
       </c>
-      <c r="CV2">
+      <c r="CS2">
         <v>-1</v>
       </c>
     </row>
@@ -1683,11 +1687,11 @@
       <c r="D3" s="1" t="s">
         <v>220</v>
       </c>
+      <c r="BT3" s="1"/>
+      <c r="BU3" s="1"/>
       <c r="BW3" s="1"/>
-      <c r="BX3" s="1"/>
-      <c r="BZ3" s="1"/>
-      <c r="CE3" s="1"/>
-      <c r="CU3" t="s">
+      <c r="CB3" s="1"/>
+      <c r="CR3" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1704,27 +1708,36 @@
       <c r="E4" t="s">
         <v>167</v>
       </c>
+      <c r="R4" t="s">
+        <v>87</v>
+      </c>
+      <c r="S4">
+        <v>887</v>
+      </c>
+      <c r="T4">
+        <v>1234</v>
+      </c>
       <c r="U4" t="s">
-        <v>87</v>
-      </c>
-      <c r="V4">
-        <v>887</v>
+        <v>168</v>
+      </c>
+      <c r="V4" t="s">
+        <v>87</v>
       </c>
       <c r="W4">
-        <v>1234</v>
-      </c>
-      <c r="X4" t="s">
-        <v>168</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z4">
         <v>381942349</v>
       </c>
-      <c r="AA4">
+      <c r="X4">
         <v>123</v>
       </c>
+      <c r="Z4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>87</v>
+      </c>
       <c r="AC4" t="s">
         <v>87</v>
       </c>
@@ -1734,29 +1747,29 @@
       <c r="AE4" t="s">
         <v>87</v>
       </c>
-      <c r="AF4" t="s">
-        <v>87</v>
+      <c r="AF4">
+        <v>94219</v>
       </c>
       <c r="AG4" t="s">
-        <v>87</v>
+        <v>169</v>
       </c>
       <c r="AH4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AI4">
-        <v>94219</v>
+        <v>170</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>87</v>
       </c>
       <c r="AJ4" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="AK4" t="s">
-        <v>170</v>
+        <v>87</v>
       </c>
       <c r="AL4" t="s">
         <v>87</v>
       </c>
       <c r="AM4" t="s">
-        <v>171</v>
+        <v>87</v>
       </c>
       <c r="AN4" t="s">
         <v>87</v>
@@ -1770,163 +1783,154 @@
       <c r="AQ4" t="s">
         <v>87</v>
       </c>
-      <c r="AR4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AU4">
+      <c r="AR4">
         <v>2130</v>
       </c>
-      <c r="AV4">
+      <c r="AS4">
         <v>12345</v>
       </c>
+      <c r="AT4">
+        <v>324899</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>172</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>174</v>
+      </c>
       <c r="AW4">
-        <v>324899</v>
+        <v>12451324</v>
       </c>
       <c r="AX4" t="s">
-        <v>172</v>
-      </c>
-      <c r="AY4" t="s">
-        <v>174</v>
-      </c>
-      <c r="AZ4">
-        <v>12451324</v>
-      </c>
-      <c r="BA4" t="s">
         <v>175</v>
       </c>
-      <c r="BB4">
+      <c r="AY4">
         <v>124394</v>
       </c>
-      <c r="BC4" t="s">
+      <c r="AZ4" t="s">
         <v>179</v>
       </c>
+      <c r="BE4" t="s">
+        <v>176</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BG4" t="s">
+        <v>180</v>
+      </c>
       <c r="BH4" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="BI4" t="s">
         <v>87</v>
       </c>
       <c r="BJ4" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="BK4" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="BL4" t="s">
-        <v>87</v>
+        <v>186</v>
       </c>
       <c r="BM4" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="BN4" t="s">
-        <v>185</v>
+        <v>87</v>
       </c>
       <c r="BO4" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="BP4" t="s">
-        <v>187</v>
+        <v>87</v>
       </c>
       <c r="BQ4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BR4" t="s">
-        <v>188</v>
-      </c>
-      <c r="BS4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BT4" t="s">
         <v>189</v>
       </c>
+      <c r="BR4" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="BS4" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="BT4" s="1" t="s">
+        <v>192</v>
+      </c>
       <c r="BU4" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="BV4" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="BW4" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="BX4" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="BY4" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
+      </c>
+      <c r="BY4" t="s">
+        <v>197</v>
       </c>
       <c r="BZ4" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="CA4" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="CB4" t="s">
-        <v>197</v>
-      </c>
-      <c r="CC4" s="1" t="s">
         <v>198</v>
       </c>
+      <c r="CA4" t="s">
+        <v>199</v>
+      </c>
+      <c r="CB4" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="CC4" t="s">
+        <v>201</v>
+      </c>
       <c r="CD4" t="s">
-        <v>199</v>
-      </c>
-      <c r="CE4" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
+      </c>
+      <c r="CE4" t="s">
+        <v>203</v>
       </c>
       <c r="CF4" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="CG4" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="CH4" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="CI4" t="s">
-        <v>204</v>
-      </c>
-      <c r="CJ4" t="s">
-        <v>205</v>
+        <v>207</v>
+      </c>
+      <c r="CJ4" s="3">
+        <v>44124</v>
       </c>
       <c r="CK4" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="CL4" t="s">
-        <v>207</v>
-      </c>
-      <c r="CM4" s="3">
-        <v>44124</v>
+        <v>209</v>
+      </c>
+      <c r="CM4" t="s">
+        <v>210</v>
       </c>
       <c r="CN4" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="CO4" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="CP4" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="CQ4" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="CR4" t="s">
-        <v>212</v>
-      </c>
-      <c r="CS4" t="s">
-        <v>213</v>
-      </c>
-      <c r="CT4" t="s">
-        <v>214</v>
-      </c>
-      <c r="CU4" t="s">
         <v>218</v>
       </c>
-      <c r="CV4">
+      <c r="CS4">
         <v>5.5</v>
       </c>
     </row>
@@ -1961,256 +1965,256 @@
       <c r="J5" t="s">
         <v>85</v>
       </c>
+      <c r="K5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M5" t="s">
+        <v>87</v>
+      </c>
       <c r="N5" t="s">
-        <v>98</v>
-      </c>
-      <c r="P5" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q5" t="s">
         <v>85</v>
       </c>
+      <c r="O5" t="s">
+        <v>87</v>
+      </c>
       <c r="R5" t="s">
         <v>87</v>
       </c>
+      <c r="S5" t="s">
+        <v>99</v>
+      </c>
+      <c r="T5" t="s">
+        <v>100</v>
+      </c>
       <c r="U5" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="V5" t="s">
+        <v>87</v>
+      </c>
+      <c r="W5" t="s">
+        <v>101</v>
+      </c>
+      <c r="X5" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF5" t="s">
         <v>99</v>
       </c>
-      <c r="W5" t="s">
+      <c r="AG5" t="s">
         <v>100</v>
       </c>
-      <c r="X5" t="s">
+      <c r="AH5" t="s">
+        <v>155</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>156</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR5" t="s">
         <v>125</v>
       </c>
-      <c r="Y5" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>101</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>128</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>99</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>100</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>155</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>156</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AR5" t="s">
-        <v>87</v>
-      </c>
       <c r="AS5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AT5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="AU5" t="s">
-        <v>125</v>
+        <v>224</v>
       </c>
       <c r="AV5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="AW5" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="AX5" t="s">
-        <v>224</v>
+        <v>102</v>
       </c>
       <c r="AY5" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="AZ5" t="s">
-        <v>127</v>
-      </c>
-      <c r="BA5" t="s">
-        <v>102</v>
-      </c>
-      <c r="BB5" t="s">
-        <v>103</v>
-      </c>
-      <c r="BC5" t="s">
         <v>91</v>
       </c>
+      <c r="BE5" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>87</v>
+      </c>
+      <c r="BG5" t="s">
+        <v>104</v>
+      </c>
       <c r="BH5" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="BI5" t="s">
         <v>87</v>
       </c>
       <c r="BJ5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="BK5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="BL5" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="BM5" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="BN5" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="BO5" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
       <c r="BP5" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="BQ5" t="s">
-        <v>87</v>
-      </c>
-      <c r="BR5" t="s">
-        <v>143</v>
-      </c>
-      <c r="BS5" t="s">
-        <v>87</v>
-      </c>
-      <c r="BT5" t="s">
         <v>110</v>
       </c>
+      <c r="BR5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BS5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BT5" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="BU5" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="BV5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="BV5" t="s">
         <v>87</v>
       </c>
       <c r="BW5" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="BX5" s="1" t="s">
+      <c r="BX5" t="s">
+        <v>87</v>
+      </c>
+      <c r="BY5" t="s">
+        <v>85</v>
+      </c>
+      <c r="BZ5" t="s">
+        <v>87</v>
+      </c>
+      <c r="CA5" t="s">
+        <v>85</v>
+      </c>
+      <c r="CB5" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="BY5" t="s">
-        <v>87</v>
-      </c>
-      <c r="BZ5" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="CA5" t="s">
-        <v>87</v>
-      </c>
-      <c r="CB5" t="s">
-        <v>85</v>
-      </c>
       <c r="CC5" t="s">
         <v>87</v>
       </c>
       <c r="CD5" t="s">
-        <v>85</v>
-      </c>
-      <c r="CE5" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="CF5" t="s">
-        <v>87</v>
-      </c>
-      <c r="CG5" t="s">
         <v>111</v>
       </c>
+      <c r="CE5" t="s">
+        <v>112</v>
+      </c>
       <c r="CH5" t="s">
-        <v>112</v>
+        <v>123</v>
+      </c>
+      <c r="CI5" t="s">
+        <v>163</v>
+      </c>
+      <c r="CJ5" t="s">
+        <v>162</v>
       </c>
       <c r="CK5" t="s">
+        <v>157</v>
+      </c>
+      <c r="CL5" t="s">
+        <v>158</v>
+      </c>
+      <c r="CM5" t="s">
+        <v>161</v>
+      </c>
+      <c r="CN5" t="s">
+        <v>160</v>
+      </c>
+      <c r="CO5" t="s">
+        <v>159</v>
+      </c>
+      <c r="CP5" t="s">
+        <v>125</v>
+      </c>
+      <c r="CQ5" t="s">
+        <v>126</v>
+      </c>
+      <c r="CR5">
         <v>123</v>
       </c>
-      <c r="CL5" t="s">
-        <v>163</v>
-      </c>
-      <c r="CM5" t="s">
-        <v>162</v>
-      </c>
-      <c r="CN5" t="s">
-        <v>157</v>
-      </c>
-      <c r="CO5" t="s">
-        <v>158</v>
-      </c>
-      <c r="CP5" t="s">
-        <v>161</v>
-      </c>
-      <c r="CQ5" t="s">
-        <v>160</v>
-      </c>
-      <c r="CR5" t="s">
-        <v>159</v>
-      </c>
       <c r="CS5" t="s">
-        <v>125</v>
-      </c>
-      <c r="CT5" t="s">
-        <v>126</v>
-      </c>
-      <c r="CU5">
-        <v>123</v>
-      </c>
-      <c r="CV5" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:102" x14ac:dyDescent="0.15">
+      <c r="BT6" s="1"/>
+      <c r="BU6" s="1"/>
       <c r="BW6" s="1"/>
-      <c r="BX6" s="1"/>
-      <c r="BZ6" s="1"/>
-      <c r="CE6" s="1"/>
+      <c r="CB6" s="1"/>
     </row>
     <row r="7" spans="1:102" x14ac:dyDescent="0.15">
       <c r="D7" s="2"/>
+      <c r="BL7" s="2"/>
+      <c r="BM7" s="2"/>
       <c r="BO7" s="2"/>
-      <c r="BP7" s="2"/>
-      <c r="BR7" s="2"/>
+      <c r="BT7" s="1"/>
+      <c r="BU7" s="1"/>
       <c r="BW7" s="1"/>
-      <c r="BX7" s="1"/>
-      <c r="BZ7" s="1"/>
-      <c r="CE7" s="1"/>
-      <c r="CK7" s="3"/>
-      <c r="CR7" s="2"/>
-      <c r="CS7" s="3"/>
+      <c r="CB7" s="1"/>
+      <c r="CH7" s="3"/>
+      <c r="CO7" s="2"/>
+      <c r="CP7" s="3"/>
     </row>
     <row r="8" spans="1:102" x14ac:dyDescent="0.15">
       <c r="F8" s="1"/>
@@ -2218,19 +2222,16 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="BU8"/>
+      <c r="N8" s="1"/>
+      <c r="BR8"/>
+      <c r="BT8" s="1"/>
+      <c r="BU8" s="1"/>
       <c r="BW8" s="1"/>
       <c r="BX8" s="1"/>
-      <c r="BZ8" s="1"/>
+      <c r="BY8" s="1"/>
       <c r="CA8" s="1"/>
       <c r="CB8" s="1"/>
       <c r="CD8" s="1"/>
-      <c r="CE8" s="1"/>
-      <c r="CG8" s="1"/>
     </row>
     <row r="9" spans="1:102" x14ac:dyDescent="0.15">
       <c r="D9" s="3"/>
@@ -2239,27 +2240,24 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="BC9" s="3"/>
-      <c r="BH9" s="3"/>
-      <c r="BU9"/>
-      <c r="CB9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="AZ9" s="3"/>
+      <c r="BE9" s="3"/>
+      <c r="BR9"/>
+      <c r="BY9" s="1"/>
+      <c r="CA9" s="1"/>
+      <c r="CC9" s="1"/>
       <c r="CD9" s="1"/>
-      <c r="CF9" s="1"/>
-      <c r="CG9" s="1"/>
     </row>
     <row r="10" spans="1:102" x14ac:dyDescent="0.15">
-      <c r="BC10" s="2"/>
-      <c r="BH10" s="2"/>
-      <c r="BR10" s="3"/>
-      <c r="CN10" s="3"/>
-      <c r="CO10" s="2"/>
-      <c r="CR10" s="3"/>
-      <c r="CS10" s="2"/>
+      <c r="AZ10" s="2"/>
+      <c r="BE10" s="2"/>
+      <c r="BO10" s="3"/>
+      <c r="CK10" s="3"/>
+      <c r="CL10" s="2"/>
+      <c r="CO10" s="3"/>
+      <c r="CP10" s="2"/>
     </row>
     <row r="12" spans="1:102" x14ac:dyDescent="0.15">
       <c r="D12" s="1"/>

</xml_diff>

<commit_message>
Refactor date validation out of import_controller
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA-ALERT/SaraAlert/test/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nfreiter\dev\sara\SaraAlert\test\fixtures\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BEAD7B-BECB-CD41-A42A-9EB2C7739FC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6105BAE-1794-4413-BF5F-394734BF2D4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="10690" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitorees" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" refMode="R1C1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="221">
   <si>
     <t>First Name</t>
   </si>
@@ -493,15 +493,6 @@
     <t>asbs</t>
   </si>
   <si>
-    <t>dfsasga</t>
-  </si>
-  <si>
-    <t>asdfasdf</t>
-  </si>
-  <si>
-    <t>asdfsfd</t>
-  </si>
-  <si>
     <t>adsf</t>
   </si>
   <si>
@@ -646,24 +637,12 @@
     <t>(W$*RU)#JFPi</t>
   </si>
   <si>
-    <t>)W$*#%R#H)E</t>
-  </si>
-  <si>
-    <t>43238u090DSF#%#</t>
-  </si>
-  <si>
     <t>#W($&amp;@R</t>
   </si>
   <si>
     <t>01/01/1000</t>
   </si>
   <si>
-    <t>05/01/600</t>
-  </si>
-  <si>
-    <t>12/12/1212</t>
-  </si>
-  <si>
     <t>a39%3</t>
   </si>
   <si>
@@ -695,6 +674,15 @@
   </si>
   <si>
     <t>333-333-3333</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>22/11/2020</t>
+  </si>
+  <si>
+    <t>12/9/2020</t>
   </si>
 </sst>
 </file>
@@ -1049,112 +1037,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CU12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="AU6" sqref="AU6"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CJ1" workbookViewId="0">
+      <selection activeCell="CP4" sqref="CP4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21.625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="18.5" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="22" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.375" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="23.125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="29" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="28.375" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="29" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="26.625" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="30" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.625" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.125" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="24" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.625" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="15" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="20.875" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="20" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="12.625" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="26.625" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="38.83203125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="36.375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="38.875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="30.625" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="30" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="34.125" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="19.5" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="24" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="21.625" style="1" bestFit="1" customWidth="1"/>
     <col min="71" max="71" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="32.83203125" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="40.625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="38.625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="30.625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="20.625" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="35.1640625" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="31.375" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="35.125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="28.625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="24.125" bestFit="1" customWidth="1"/>
     <col min="83" max="83" width="38" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="13.125" bestFit="1" customWidth="1"/>
     <col min="88" max="88" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="17.625" bestFit="1" customWidth="1"/>
     <col min="91" max="91" width="12" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="27.375" bestFit="1" customWidth="1"/>
     <col min="94" max="94" width="16" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="12" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="26.125" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1441,21 +1429,21 @@
         <v>122</v>
       </c>
       <c r="CR1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="CS1" t="s">
+        <v>208</v>
+      </c>
+      <c r="CT1" t="s">
         <v>215</v>
       </c>
-      <c r="CT1" t="s">
-        <v>222</v>
-      </c>
       <c r="CU1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.2">
       <c r="D2" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="E2" t="s">
         <v>125</v>
@@ -1548,7 +1536,7 @@
         <v>138</v>
       </c>
       <c r="AV2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="AW2" t="s">
         <v>139</v>
@@ -1557,22 +1545,22 @@
         <v>140</v>
       </c>
       <c r="AZ2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="BE2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="BF2" t="s">
         <v>87</v>
       </c>
       <c r="BG2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="BH2" t="s">
         <v>87</v>
       </c>
       <c r="BI2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="BJ2" t="s">
         <v>87</v>
@@ -1660,9 +1648,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.2">
       <c r="D3" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="BT3" s="1"/>
       <c r="BU3" s="1"/>
@@ -1672,18 +1660,18 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D4" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="R4" t="s">
         <v>87</v>
@@ -1695,7 +1683,7 @@
         <v>1234</v>
       </c>
       <c r="U4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="V4" t="s">
         <v>87</v>
@@ -1728,16 +1716,16 @@
         <v>94219</v>
       </c>
       <c r="AG4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AH4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="AI4" t="s">
         <v>87</v>
       </c>
       <c r="AJ4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="AK4" t="s">
         <v>87</v>
@@ -1770,148 +1758,148 @@
         <v>324899</v>
       </c>
       <c r="AU4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="AV4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AW4">
         <v>12451324</v>
       </c>
       <c r="AX4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AY4">
         <v>124394</v>
       </c>
       <c r="AZ4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="BE4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="BF4" t="s">
         <v>87</v>
       </c>
       <c r="BG4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="BH4" t="s">
+        <v>178</v>
+      </c>
+      <c r="BI4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BJ4" t="s">
         <v>181</v>
       </c>
-      <c r="BI4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BJ4" t="s">
+      <c r="BK4" t="s">
+        <v>182</v>
+      </c>
+      <c r="BL4" t="s">
+        <v>183</v>
+      </c>
+      <c r="BM4" t="s">
         <v>184</v>
       </c>
-      <c r="BK4" t="s">
+      <c r="BN4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BO4" t="s">
         <v>185</v>
       </c>
-      <c r="BL4" t="s">
+      <c r="BP4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BQ4" t="s">
         <v>186</v>
       </c>
-      <c r="BM4" t="s">
+      <c r="BR4" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="BN4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BO4" t="s">
+      <c r="BS4" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="BP4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BQ4" t="s">
+      <c r="BT4" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="BR4" s="1" t="s">
+      <c r="BU4" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BS4" s="1" t="s">
+      <c r="BV4" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BT4" s="1" t="s">
+      <c r="BW4" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="BU4" s="1" t="s">
+      <c r="BX4" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BV4" s="1" t="s">
+      <c r="BY4" t="s">
         <v>194</v>
       </c>
-      <c r="BW4" s="1" t="s">
+      <c r="BZ4" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="BX4" s="1" t="s">
+      <c r="CA4" t="s">
         <v>196</v>
       </c>
-      <c r="BY4" t="s">
+      <c r="CB4" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="BZ4" s="1" t="s">
+      <c r="CC4" t="s">
         <v>198</v>
       </c>
-      <c r="CA4" t="s">
+      <c r="CD4" t="s">
         <v>199</v>
       </c>
-      <c r="CB4" s="1" t="s">
+      <c r="CE4" t="s">
         <v>200</v>
       </c>
-      <c r="CC4" t="s">
+      <c r="CF4" t="s">
         <v>201</v>
       </c>
-      <c r="CD4" t="s">
+      <c r="CG4" t="s">
         <v>202</v>
       </c>
-      <c r="CE4" t="s">
+      <c r="CH4" t="s">
         <v>203</v>
       </c>
-      <c r="CF4" t="s">
+      <c r="CI4" t="s">
         <v>204</v>
-      </c>
-      <c r="CG4" t="s">
-        <v>205</v>
-      </c>
-      <c r="CH4" t="s">
-        <v>206</v>
-      </c>
-      <c r="CI4" t="s">
-        <v>207</v>
       </c>
       <c r="CJ4" s="3">
         <v>44124</v>
       </c>
-      <c r="CK4" t="s">
-        <v>208</v>
-      </c>
-      <c r="CL4" t="s">
-        <v>209</v>
+      <c r="CK4" s="2">
+        <v>44174</v>
+      </c>
+      <c r="CL4" s="2">
+        <v>44174</v>
       </c>
       <c r="CM4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="CN4" t="s">
+        <v>206</v>
+      </c>
+      <c r="CO4" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="CP4" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="CQ4" t="s">
+        <v>207</v>
+      </c>
+      <c r="CR4" t="s">
         <v>211</v>
-      </c>
-      <c r="CO4" t="s">
-        <v>212</v>
-      </c>
-      <c r="CP4" t="s">
-        <v>213</v>
-      </c>
-      <c r="CQ4" t="s">
-        <v>214</v>
-      </c>
-      <c r="CR4" t="s">
-        <v>218</v>
       </c>
       <c r="CS4">
         <v>5.5</v>
       </c>
     </row>
-    <row r="5" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -1922,7 +1910,7 @@
         <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E5" t="s">
         <v>97</v>
@@ -2039,7 +2027,7 @@
         <v>89</v>
       </c>
       <c r="AU5" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="AV5" t="s">
         <v>90</v>
@@ -2141,28 +2129,28 @@
         <v>123</v>
       </c>
       <c r="CI5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="CJ5" t="s">
-        <v>162</v>
-      </c>
-      <c r="CK5" t="s">
+        <v>159</v>
+      </c>
+      <c r="CK5" s="2">
+        <v>44174</v>
+      </c>
+      <c r="CL5" s="2">
+        <v>44174</v>
+      </c>
+      <c r="CM5" t="s">
+        <v>158</v>
+      </c>
+      <c r="CN5" t="s">
         <v>157</v>
       </c>
-      <c r="CL5" t="s">
-        <v>158</v>
-      </c>
-      <c r="CM5" t="s">
-        <v>161</v>
-      </c>
-      <c r="CN5" t="s">
-        <v>160</v>
-      </c>
-      <c r="CO5" t="s">
-        <v>159</v>
-      </c>
-      <c r="CP5" t="s">
-        <v>125</v>
+      <c r="CO5" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="CP5" s="1">
+        <v>44174</v>
       </c>
       <c r="CQ5" t="s">
         <v>126</v>
@@ -2171,16 +2159,16 @@
         <v>123</v>
       </c>
       <c r="CS5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:99" x14ac:dyDescent="0.2">
       <c r="BT6" s="1"/>
       <c r="BU6" s="1"/>
       <c r="BW6" s="1"/>
       <c r="CB6" s="1"/>
     </row>
-    <row r="7" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:99" x14ac:dyDescent="0.2">
       <c r="D7" s="2"/>
       <c r="BL7" s="2"/>
       <c r="BM7" s="2"/>
@@ -2193,7 +2181,7 @@
       <c r="CO7" s="2"/>
       <c r="CP7" s="3"/>
     </row>
-    <row r="8" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:99" x14ac:dyDescent="0.2">
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -2210,7 +2198,7 @@
       <c r="CB8" s="1"/>
       <c r="CD8" s="1"/>
     </row>
-    <row r="9" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:99" x14ac:dyDescent="0.2">
       <c r="D9" s="3"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -2227,7 +2215,7 @@
       <c r="CC9" s="1"/>
       <c r="CD9" s="1"/>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:99" x14ac:dyDescent="0.2">
       <c r="AZ10" s="2"/>
       <c r="BE10" s="2"/>
       <c r="BO10" s="3"/>
@@ -2236,12 +2224,12 @@
       <c r="CO10" s="3"/>
       <c r="CP10" s="2"/>
     </row>
-    <row r="12" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:99" x14ac:dyDescent="0.2">
       <c r="D12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="D3" twoDigitTextYear="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
Revert unintentional change to Excel file
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nfreiter\dev\sara\SaraAlert\test\fixtures\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA-ALERT/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6105BAE-1794-4413-BF5F-394734BF2D4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BEAD7B-BECB-CD41-A42A-9EB2C7739FC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="10690" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitorees" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="225">
   <si>
     <t>First Name</t>
   </si>
@@ -493,6 +493,15 @@
     <t>asbs</t>
   </si>
   <si>
+    <t>dfsasga</t>
+  </si>
+  <si>
+    <t>asdfasdf</t>
+  </si>
+  <si>
+    <t>asdfsfd</t>
+  </si>
+  <si>
     <t>adsf</t>
   </si>
   <si>
@@ -637,12 +646,24 @@
     <t>(W$*RU)#JFPi</t>
   </si>
   <si>
+    <t>)W$*#%R#H)E</t>
+  </si>
+  <si>
+    <t>43238u090DSF#%#</t>
+  </si>
+  <si>
     <t>#W($&amp;@R</t>
   </si>
   <si>
     <t>01/01/1000</t>
   </si>
   <si>
+    <t>05/01/600</t>
+  </si>
+  <si>
+    <t>12/12/1212</t>
+  </si>
+  <si>
     <t>a39%3</t>
   </si>
   <si>
@@ -674,15 +695,6 @@
   </si>
   <si>
     <t>333-333-3333</t>
-  </si>
-  <si>
-    <t>foo</t>
-  </si>
-  <si>
-    <t>22/11/2020</t>
-  </si>
-  <si>
-    <t>12/9/2020</t>
   </si>
 </sst>
 </file>
@@ -1037,112 +1049,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CU12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CJ1" workbookViewId="0">
-      <selection activeCell="CP4" sqref="CP4"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="AU6" sqref="AU6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="18.5" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="22" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="22.125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="29" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="29" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="30" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="24" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="20.375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="27.875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="15" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="20" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="19.125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="36.375" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="38.875" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="30.625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="30" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="34.1640625" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="19.5" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="24" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="23.625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="21.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="71" max="71" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="32.875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="40.625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="38.625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="30.625" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="31.375" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="35.125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="28.625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="83" max="83" width="38" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="26.375" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="88" max="88" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="91" max="91" width="12" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="94" max="94" width="16" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="12" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:99" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1429,21 +1441,21 @@
         <v>122</v>
       </c>
       <c r="CR1" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="CS1" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="CT1" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="CU1" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.15">
       <c r="D2" s="1" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="E2" t="s">
         <v>125</v>
@@ -1536,7 +1548,7 @@
         <v>138</v>
       </c>
       <c r="AV2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="AW2" t="s">
         <v>139</v>
@@ -1545,22 +1557,22 @@
         <v>140</v>
       </c>
       <c r="AZ2" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="BE2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="BF2" t="s">
         <v>87</v>
       </c>
       <c r="BG2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="BH2" t="s">
         <v>87</v>
       </c>
       <c r="BI2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="BJ2" t="s">
         <v>87</v>
@@ -1648,9 +1660,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.15">
       <c r="D3" s="1" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="BT3" s="1"/>
       <c r="BU3" s="1"/>
@@ -1660,18 +1672,18 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C4" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D4" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="E4" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="R4" t="s">
         <v>87</v>
@@ -1683,7 +1695,7 @@
         <v>1234</v>
       </c>
       <c r="U4" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="V4" t="s">
         <v>87</v>
@@ -1716,16 +1728,16 @@
         <v>94219</v>
       </c>
       <c r="AG4" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="AH4" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="AI4" t="s">
         <v>87</v>
       </c>
       <c r="AJ4" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="AK4" t="s">
         <v>87</v>
@@ -1758,148 +1770,148 @@
         <v>324899</v>
       </c>
       <c r="AU4" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="AV4" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="AW4">
         <v>12451324</v>
       </c>
       <c r="AX4" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="AY4">
         <v>124394</v>
       </c>
       <c r="AZ4" t="s">
+        <v>179</v>
+      </c>
+      <c r="BE4" t="s">
         <v>176</v>
       </c>
-      <c r="BE4" t="s">
-        <v>173</v>
-      </c>
       <c r="BF4" t="s">
         <v>87</v>
       </c>
       <c r="BG4" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="BH4" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="BI4" t="s">
         <v>87</v>
       </c>
       <c r="BJ4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="BK4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="BL4" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="BM4" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="BN4" t="s">
         <v>87</v>
       </c>
       <c r="BO4" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="BP4" t="s">
         <v>87</v>
       </c>
       <c r="BQ4" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="BR4" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="BS4" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="BT4" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="BU4" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="BV4" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="BW4" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="BX4" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="BY4" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="BZ4" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="CA4" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="CB4" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="CC4" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="CD4" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="CE4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="CF4" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="CG4" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="CH4" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="CI4" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="CJ4" s="3">
         <v>44124</v>
       </c>
-      <c r="CK4" s="2">
-        <v>44174</v>
-      </c>
-      <c r="CL4" s="2">
-        <v>44174</v>
+      <c r="CK4" t="s">
+        <v>208</v>
+      </c>
+      <c r="CL4" t="s">
+        <v>209</v>
       </c>
       <c r="CM4" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="CN4" t="s">
-        <v>206</v>
-      </c>
-      <c r="CO4" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="CO4" t="s">
+        <v>212</v>
+      </c>
+      <c r="CP4" t="s">
+        <v>213</v>
+      </c>
+      <c r="CQ4" t="s">
+        <v>214</v>
+      </c>
+      <c r="CR4" t="s">
         <v>218</v>
-      </c>
-      <c r="CP4" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="CQ4" t="s">
-        <v>207</v>
-      </c>
-      <c r="CR4" t="s">
-        <v>211</v>
       </c>
       <c r="CS4">
         <v>5.5</v>
       </c>
     </row>
-    <row r="5" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:99" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -1910,7 +1922,7 @@
         <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="E5" t="s">
         <v>97</v>
@@ -2027,7 +2039,7 @@
         <v>89</v>
       </c>
       <c r="AU5" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="AV5" t="s">
         <v>90</v>
@@ -2129,28 +2141,28 @@
         <v>123</v>
       </c>
       <c r="CI5" t="s">
+        <v>163</v>
+      </c>
+      <c r="CJ5" t="s">
+        <v>162</v>
+      </c>
+      <c r="CK5" t="s">
+        <v>157</v>
+      </c>
+      <c r="CL5" t="s">
+        <v>158</v>
+      </c>
+      <c r="CM5" t="s">
+        <v>161</v>
+      </c>
+      <c r="CN5" t="s">
         <v>160</v>
       </c>
-      <c r="CJ5" t="s">
+      <c r="CO5" t="s">
         <v>159</v>
       </c>
-      <c r="CK5" s="2">
-        <v>44174</v>
-      </c>
-      <c r="CL5" s="2">
-        <v>44174</v>
-      </c>
-      <c r="CM5" t="s">
-        <v>158</v>
-      </c>
-      <c r="CN5" t="s">
-        <v>157</v>
-      </c>
-      <c r="CO5" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="CP5" s="1">
-        <v>44174</v>
+      <c r="CP5" t="s">
+        <v>125</v>
       </c>
       <c r="CQ5" t="s">
         <v>126</v>
@@ -2159,16 +2171,16 @@
         <v>123</v>
       </c>
       <c r="CS5" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:99" x14ac:dyDescent="0.15">
       <c r="BT6" s="1"/>
       <c r="BU6" s="1"/>
       <c r="BW6" s="1"/>
       <c r="CB6" s="1"/>
     </row>
-    <row r="7" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:99" x14ac:dyDescent="0.15">
       <c r="D7" s="2"/>
       <c r="BL7" s="2"/>
       <c r="BM7" s="2"/>
@@ -2181,7 +2193,7 @@
       <c r="CO7" s="2"/>
       <c r="CP7" s="3"/>
     </row>
-    <row r="8" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:99" x14ac:dyDescent="0.15">
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -2198,7 +2210,7 @@
       <c r="CB8" s="1"/>
       <c r="CD8" s="1"/>
     </row>
-    <row r="9" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:99" x14ac:dyDescent="0.15">
       <c r="D9" s="3"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -2215,7 +2227,7 @@
       <c r="CC9" s="1"/>
       <c r="CD9" s="1"/>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:99" x14ac:dyDescent="0.15">
       <c r="AZ10" s="2"/>
       <c r="BE10" s="2"/>
       <c r="BO10" s="3"/>
@@ -2224,12 +2236,12 @@
       <c r="CO10" s="3"/>
       <c r="CP10" s="2"/>
     </row>
-    <row r="12" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:99" x14ac:dyDescent="0.15">
       <c r="D12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <ignoredErrors>
     <ignoredError sqref="D3" twoDigitTextYear="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
validate follow_up_note and update formatting guidance release date
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA-ALERT/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14D5792-C6AE-5B46-AEF4-B3679A1406FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF5F0C4-F69B-444E-B462-29C1158648B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="258">
   <si>
     <t>First Name</t>
   </si>
@@ -791,6 +791,9 @@
   </si>
   <si>
     <t>invalid reason</t>
+  </si>
+  <si>
+    <t>note</t>
   </si>
 </sst>
 </file>
@@ -1889,6 +1892,9 @@
       <c r="DH3" t="s">
         <v>252</v>
       </c>
+      <c r="DJ3" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="4" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A4" t="s">

</xml_diff>

<commit_message>
use formatted preferred contact times for import/export and format select input
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA-ALERT/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF5F0C4-F69B-444E-B462-29C1158648B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BB7129-8052-EC4D-BB64-AD19C99A6D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="259">
   <si>
     <t>First Name</t>
   </si>
@@ -403,9 +403,6 @@
     <t>fdsa</t>
   </si>
   <si>
-    <t>Morning</t>
-  </si>
-  <si>
     <t>County 1</t>
   </si>
   <si>
@@ -794,6 +791,12 @@
   </si>
   <si>
     <t>note</t>
+  </si>
+  <si>
+    <t>24:00</t>
+  </si>
+  <si>
+    <t>1:30</t>
   </si>
 </sst>
 </file>
@@ -1199,7 +1202,7 @@
     <col min="46" max="46" width="21.5" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="24" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="15.6640625" bestFit="1" customWidth="1"/>
@@ -1412,7 +1415,7 @@
       <c r="AV1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>48</v>
       </c>
       <c r="AX1" t="s">
@@ -1554,66 +1557,66 @@
         <v>122</v>
       </c>
       <c r="CR1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="CS1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="CT1" t="s">
+        <v>221</v>
+      </c>
+      <c r="CU1" t="s">
         <v>222</v>
       </c>
-      <c r="CU1" t="s">
-        <v>223</v>
-      </c>
       <c r="CV1" t="s">
+        <v>225</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>224</v>
+      </c>
+      <c r="CX1" t="s">
         <v>226</v>
       </c>
-      <c r="CW1" t="s">
-        <v>225</v>
-      </c>
-      <c r="CX1" t="s">
+      <c r="CY1" t="s">
         <v>227</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="CZ1" t="s">
         <v>228</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DA1" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DB1" t="s">
         <v>230</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DC1" t="s">
         <v>231</v>
       </c>
-      <c r="DC1" t="s">
+      <c r="DD1" t="s">
         <v>232</v>
       </c>
-      <c r="DD1" t="s">
+      <c r="DE1" t="s">
         <v>233</v>
       </c>
-      <c r="DE1" t="s">
+      <c r="DF1" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="DF1" s="1" t="s">
+      <c r="DG1" t="s">
         <v>235</v>
       </c>
-      <c r="DG1" t="s">
+      <c r="DH1" t="s">
         <v>236</v>
       </c>
-      <c r="DH1" t="s">
-        <v>237</v>
-      </c>
       <c r="DI1" t="s">
+        <v>253</v>
+      </c>
+      <c r="DJ1" t="s">
         <v>254</v>
-      </c>
-      <c r="DJ1" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:114" x14ac:dyDescent="0.15">
       <c r="D2" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E2" t="s">
         <v>125</v>
@@ -1622,127 +1625,127 @@
         <v>126</v>
       </c>
       <c r="G2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" t="s">
         <v>129</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J2" t="s">
         <v>130</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
+        <v>131</v>
+      </c>
+      <c r="M2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" t="s">
         <v>133</v>
       </c>
-      <c r="J2" t="s">
-        <v>131</v>
-      </c>
-      <c r="K2" t="s">
-        <v>132</v>
-      </c>
-      <c r="M2" t="s">
-        <v>87</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
+        <v>87</v>
+      </c>
+      <c r="R2" t="s">
+        <v>87</v>
+      </c>
+      <c r="X2" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR2" t="s">
         <v>134</v>
       </c>
-      <c r="O2" t="s">
-        <v>87</v>
-      </c>
-      <c r="R2" t="s">
-        <v>87</v>
-      </c>
-      <c r="X2" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>135</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
         <v>136</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AU2" t="s">
         <v>137</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AV2" t="s">
+        <v>172</v>
+      </c>
+      <c r="AW2" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="AV2" t="s">
-        <v>173</v>
-      </c>
-      <c r="AW2" t="s">
+      <c r="AX2" t="s">
         <v>139</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="AZ2" t="s">
+        <v>177</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>176</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>182</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>181</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BL2" t="s">
         <v>140</v>
       </c>
-      <c r="AZ2" t="s">
-        <v>178</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>177</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>183</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>182</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BL2" t="s">
+      <c r="BM2" t="s">
         <v>141</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>142</v>
       </c>
       <c r="BN2" t="s">
         <v>87</v>
@@ -1755,49 +1758,49 @@
         <v>93</v>
       </c>
       <c r="BR2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="BS2" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="BS2" s="1" t="s">
+      <c r="BT2" t="s">
         <v>145</v>
       </c>
-      <c r="BT2" t="s">
+      <c r="BU2" t="s">
         <v>146</v>
       </c>
-      <c r="BU2" t="s">
+      <c r="BV2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BW2" t="s">
         <v>147</v>
       </c>
-      <c r="BV2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BW2" t="s">
+      <c r="BX2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BY2" t="s">
         <v>148</v>
       </c>
-      <c r="BX2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BY2" t="s">
+      <c r="BZ2" t="s">
+        <v>87</v>
+      </c>
+      <c r="CA2" t="s">
         <v>149</v>
       </c>
-      <c r="BZ2" t="s">
-        <v>87</v>
-      </c>
-      <c r="CA2" t="s">
+      <c r="CB2" t="s">
         <v>150</v>
       </c>
-      <c r="CB2" t="s">
+      <c r="CC2" t="s">
+        <v>87</v>
+      </c>
+      <c r="CD2" t="s">
         <v>151</v>
       </c>
-      <c r="CC2" t="s">
-        <v>87</v>
-      </c>
-      <c r="CD2" t="s">
+      <c r="CE2" t="s">
         <v>152</v>
       </c>
-      <c r="CE2" t="s">
+      <c r="CH2" t="s">
         <v>153</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>154</v>
       </c>
       <c r="CJ2" t="s">
         <v>87</v>
@@ -1818,96 +1821,99 @@
         <v>-1</v>
       </c>
       <c r="CY2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="CZ2">
         <v>456</v>
       </c>
       <c r="DA2" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="DB2">
         <v>0</v>
       </c>
       <c r="DC2" t="s">
+        <v>241</v>
+      </c>
+      <c r="DD2" t="s">
         <v>242</v>
       </c>
-      <c r="DD2" t="s">
-        <v>243</v>
-      </c>
       <c r="DE2" t="s">
+        <v>245</v>
+      </c>
+      <c r="DF2" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="DF2" s="1" t="s">
-        <v>247</v>
-      </c>
       <c r="DG2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="DH2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="DI2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:114" x14ac:dyDescent="0.15">
       <c r="D3" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
+      </c>
+      <c r="AW3" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="BT3" s="1"/>
       <c r="BU3" s="1"/>
       <c r="BW3" s="1"/>
       <c r="CB3" s="1"/>
       <c r="CR3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="CY3">
         <v>123</v>
       </c>
       <c r="CZ3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="DA3" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="DB3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DC3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="DD3" t="s">
+        <v>243</v>
+      </c>
+      <c r="DE3" t="s">
         <v>244</v>
       </c>
-      <c r="DE3" t="s">
-        <v>245</v>
-      </c>
       <c r="DF3" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="DG3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="DH3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="DJ3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:114" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" t="s">
         <v>165</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>220</v>
+      </c>
+      <c r="E4" t="s">
         <v>166</v>
-      </c>
-      <c r="D4" t="s">
-        <v>221</v>
-      </c>
-      <c r="E4" t="s">
-        <v>167</v>
       </c>
       <c r="R4" t="s">
         <v>87</v>
@@ -1919,7 +1925,7 @@
         <v>1234</v>
       </c>
       <c r="U4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="V4" t="s">
         <v>87</v>
@@ -1952,16 +1958,16 @@
         <v>94219</v>
       </c>
       <c r="AG4" t="s">
+        <v>168</v>
+      </c>
+      <c r="AH4" t="s">
         <v>169</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ4" t="s">
         <v>170</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>171</v>
       </c>
       <c r="AK4" t="s">
         <v>87</v>
@@ -1994,142 +2000,142 @@
         <v>324899</v>
       </c>
       <c r="AU4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AV4" t="s">
+        <v>173</v>
+      </c>
+      <c r="AW4" s="1">
+        <v>12451324</v>
+      </c>
+      <c r="AX4" t="s">
         <v>174</v>
-      </c>
-      <c r="AW4">
-        <v>12451324</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>175</v>
       </c>
       <c r="AY4">
         <v>124394</v>
       </c>
       <c r="AZ4" t="s">
+        <v>178</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>175</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BG4" t="s">
         <v>179</v>
       </c>
-      <c r="BE4" t="s">
-        <v>176</v>
-      </c>
-      <c r="BF4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BG4" t="s">
+      <c r="BH4" t="s">
         <v>180</v>
       </c>
-      <c r="BH4" t="s">
-        <v>181</v>
-      </c>
       <c r="BI4" t="s">
         <v>87</v>
       </c>
       <c r="BJ4" t="s">
+        <v>183</v>
+      </c>
+      <c r="BK4" t="s">
         <v>184</v>
       </c>
-      <c r="BK4" t="s">
+      <c r="BL4" t="s">
         <v>185</v>
       </c>
-      <c r="BL4" t="s">
+      <c r="BM4" t="s">
         <v>186</v>
       </c>
-      <c r="BM4" t="s">
+      <c r="BN4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BO4" t="s">
         <v>187</v>
       </c>
-      <c r="BN4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BO4" t="s">
+      <c r="BP4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BQ4" t="s">
         <v>188</v>
       </c>
-      <c r="BP4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BQ4" t="s">
+      <c r="BR4" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="BR4" s="1" t="s">
+      <c r="BS4" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BS4" s="1" t="s">
+      <c r="BT4" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BT4" s="1" t="s">
+      <c r="BU4" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="BU4" s="1" t="s">
+      <c r="BV4" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BV4" s="1" t="s">
+      <c r="BW4" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BW4" s="1" t="s">
+      <c r="BX4" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="BX4" s="1" t="s">
+      <c r="BY4" t="s">
         <v>196</v>
       </c>
-      <c r="BY4" t="s">
+      <c r="BZ4" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="BZ4" s="1" t="s">
+      <c r="CA4" t="s">
         <v>198</v>
       </c>
-      <c r="CA4" t="s">
+      <c r="CB4" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="CB4" s="1" t="s">
+      <c r="CC4" t="s">
         <v>200</v>
       </c>
-      <c r="CC4" t="s">
+      <c r="CD4" t="s">
         <v>201</v>
       </c>
-      <c r="CD4" t="s">
+      <c r="CE4" t="s">
         <v>202</v>
       </c>
-      <c r="CE4" t="s">
+      <c r="CF4" t="s">
         <v>203</v>
       </c>
-      <c r="CF4" t="s">
+      <c r="CG4" t="s">
         <v>204</v>
       </c>
-      <c r="CG4" t="s">
+      <c r="CH4" t="s">
         <v>205</v>
       </c>
-      <c r="CH4" t="s">
+      <c r="CI4" t="s">
         <v>206</v>
-      </c>
-      <c r="CI4" t="s">
-        <v>207</v>
       </c>
       <c r="CJ4" s="3">
         <v>44124</v>
       </c>
       <c r="CK4" t="s">
+        <v>207</v>
+      </c>
+      <c r="CL4" t="s">
         <v>208</v>
       </c>
-      <c r="CL4" t="s">
+      <c r="CM4" t="s">
         <v>209</v>
       </c>
-      <c r="CM4" t="s">
+      <c r="CN4" t="s">
         <v>210</v>
       </c>
-      <c r="CN4" t="s">
+      <c r="CO4" t="s">
         <v>211</v>
       </c>
-      <c r="CO4" t="s">
+      <c r="CP4" t="s">
         <v>212</v>
       </c>
-      <c r="CP4" t="s">
+      <c r="CQ4" t="s">
         <v>213</v>
       </c>
-      <c r="CQ4" t="s">
-        <v>214</v>
-      </c>
       <c r="CR4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="CS4">
         <v>5.5</v>
@@ -2146,7 +2152,7 @@
         <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E5" t="s">
         <v>97</v>
@@ -2197,7 +2203,7 @@
         <v>101</v>
       </c>
       <c r="X5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Z5" t="s">
         <v>87</v>
@@ -2224,13 +2230,13 @@
         <v>100</v>
       </c>
       <c r="AH5" t="s">
+        <v>154</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ5" t="s">
         <v>155</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>156</v>
       </c>
       <c r="AK5" t="s">
         <v>87</v>
@@ -2263,13 +2269,13 @@
         <v>89</v>
       </c>
       <c r="AU5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AV5" t="s">
         <v>90</v>
       </c>
-      <c r="AW5" t="s">
-        <v>127</v>
+      <c r="AW5" s="1" t="s">
+        <v>257</v>
       </c>
       <c r="AX5" t="s">
         <v>102</v>
@@ -2311,7 +2317,7 @@
         <v>87</v>
       </c>
       <c r="BO5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BP5" t="s">
         <v>87</v>
@@ -2365,25 +2371,25 @@
         <v>123</v>
       </c>
       <c r="CI5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="CJ5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="CK5" t="s">
+        <v>156</v>
+      </c>
+      <c r="CL5" t="s">
         <v>157</v>
       </c>
-      <c r="CL5" t="s">
+      <c r="CM5" t="s">
+        <v>160</v>
+      </c>
+      <c r="CN5" t="s">
+        <v>159</v>
+      </c>
+      <c r="CO5" t="s">
         <v>158</v>
-      </c>
-      <c r="CM5" t="s">
-        <v>161</v>
-      </c>
-      <c r="CN5" t="s">
-        <v>160</v>
-      </c>
-      <c r="CO5" t="s">
-        <v>159</v>
       </c>
       <c r="CP5" t="s">
         <v>125</v>
@@ -2395,7 +2401,7 @@
         <v>123</v>
       </c>
       <c r="CS5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:114" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
update test fixtures with more edge cases
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Invalid-Fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA-ALERT/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BB7129-8052-EC4D-BB64-AD19C99A6D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7DC803-A4BA-034A-B171-8BDC95F7BB9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="259">
   <si>
     <t>First Name</t>
   </si>
@@ -793,10 +793,10 @@
     <t>note</t>
   </si>
   <si>
-    <t>24:00</t>
-  </si>
-  <si>
     <t>1:30</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -830,11 +830,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1151,7 +1154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DJ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" zoomScale="91" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1859,7 +1862,7 @@
         <v>219</v>
       </c>
       <c r="AW3" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BT3" s="1"/>
       <c r="BU3" s="1"/>
@@ -2005,8 +2008,8 @@
       <c r="AV4" t="s">
         <v>173</v>
       </c>
-      <c r="AW4" s="1">
-        <v>12451324</v>
+      <c r="AW4" s="5">
+        <v>16</v>
       </c>
       <c r="AX4" t="s">
         <v>174</v>
@@ -2274,8 +2277,8 @@
       <c r="AV5" t="s">
         <v>90</v>
       </c>
-      <c r="AW5" s="1" t="s">
-        <v>257</v>
+      <c r="AW5" s="4">
+        <v>0</v>
       </c>
       <c r="AX5" t="s">
         <v>102</v>
@@ -2405,23 +2408,226 @@
       </c>
     </row>
     <row r="6" spans="1:114" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I6" t="s">
+        <v>86</v>
+      </c>
+      <c r="J6" t="s">
+        <v>85</v>
+      </c>
+      <c r="K6" t="s">
+        <v>98</v>
+      </c>
+      <c r="M6" t="s">
+        <v>87</v>
+      </c>
+      <c r="N6" t="s">
+        <v>85</v>
+      </c>
+      <c r="O6" t="s">
+        <v>87</v>
+      </c>
+      <c r="R6" t="s">
+        <v>87</v>
+      </c>
+      <c r="S6" t="s">
+        <v>99</v>
+      </c>
+      <c r="T6" t="s">
+        <v>100</v>
+      </c>
+      <c r="V6" t="s">
+        <v>87</v>
+      </c>
+      <c r="W6" t="s">
+        <v>101</v>
+      </c>
+      <c r="X6" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>88</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AW6" s="6">
+        <v>1</v>
+      </c>
       <c r="BT6" s="1"/>
       <c r="BU6" s="1"/>
       <c r="BW6" s="1"/>
       <c r="CB6" s="1"/>
     </row>
     <row r="7" spans="1:114" x14ac:dyDescent="0.15">
-      <c r="D7" s="2"/>
-      <c r="BL7" s="2"/>
-      <c r="BM7" s="2"/>
-      <c r="BO7" s="2"/>
+      <c r="A7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" t="s">
+        <v>85</v>
+      </c>
+      <c r="K7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M7" t="s">
+        <v>87</v>
+      </c>
+      <c r="N7" t="s">
+        <v>85</v>
+      </c>
+      <c r="O7" t="s">
+        <v>87</v>
+      </c>
+      <c r="R7" t="s">
+        <v>87</v>
+      </c>
+      <c r="S7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T7" t="s">
+        <v>100</v>
+      </c>
+      <c r="V7" t="s">
+        <v>87</v>
+      </c>
+      <c r="W7" t="s">
+        <v>101</v>
+      </c>
+      <c r="X7" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>88</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>89</v>
+      </c>
+      <c r="AW7" s="1" t="s">
+        <v>258</v>
+      </c>
       <c r="BT7" s="1"/>
       <c r="BU7" s="1"/>
       <c r="BW7" s="1"/>
       <c r="CB7" s="1"/>
-      <c r="CH7" s="3"/>
-      <c r="CO7" s="2"/>
-      <c r="CP7" s="3"/>
     </row>
     <row r="8" spans="1:114" x14ac:dyDescent="0.15">
       <c r="F8" s="1"/>

</xml_diff>